<commit_message>
Added final verification plots (v0.20)
</commit_message>
<xml_diff>
--- a/modules/nowcast-model/nowcast-model-inputs.xlsx
+++ b/modules/nowcast-model/nowcast-model-inputs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\modules\nowcast-model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{347DD06E-66EF-4848-B7CB-05299C962FAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1D374F7-9875-4846-B3FD-FFE201F658B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1454" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1275" uniqueCount="427">
   <si>
     <t>gdp</t>
   </si>
@@ -795,25 +795,10 @@
     <t>nc_dfm_input</t>
   </si>
   <si>
-    <t>initial_forecast</t>
-  </si>
-  <si>
     <t>nc_method</t>
   </si>
   <si>
-    <t>qual</t>
-  </si>
-  <si>
     <t>disporder</t>
-  </si>
-  <si>
-    <t>core_structural</t>
-  </si>
-  <si>
-    <t>core.endog</t>
-  </si>
-  <si>
-    <t>core.exog</t>
   </si>
   <si>
     <t>BEA.GDP</t>
@@ -1187,21 +1172,6 @@
   </si>
   <si>
     <t>Bank Real Estate Loans</t>
-  </si>
-  <si>
-    <t>post.endog</t>
-  </si>
-  <si>
-    <t>core_endog_type</t>
-  </si>
-  <si>
-    <t>identity.ll</t>
-  </si>
-  <si>
-    <t>estimated</t>
-  </si>
-  <si>
-    <t>core.exog.p</t>
   </si>
   <si>
     <t>diff1</t>
@@ -1425,214 +1395,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="44">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9393"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE4D2F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFA7FBF9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7D7D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="30">
     <dxf>
       <font>
         <strike val="0"/>
@@ -1951,6 +1714,83 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7D7D"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -1976,29 +1816,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{4AECC335-00AC-41E6-A3CA-F63691B92F69}" name="Table13279" displayName="Table13279" ref="A1:T88" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
-  <autoFilter ref="A1:T88" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
-  <tableColumns count="20">
-    <tableColumn id="1" xr3:uid="{CA6DE630-5CD5-428A-8439-1A504496E546}" name="varname" dataDxfId="41"/>
-    <tableColumn id="9" xr3:uid="{62B19A4C-5AC5-4FBE-B49F-BB64B9102385}" name="fullname" dataDxfId="40"/>
-    <tableColumn id="15" xr3:uid="{D22B03C4-4AE3-48C2-A598-07C9E704433D}" name="dispgroup" dataDxfId="39"/>
-    <tableColumn id="24" xr3:uid="{FDF2E866-66A2-44DE-B360-10560B9D2BFE}" name="disprank" dataDxfId="38"/>
-    <tableColumn id="25" xr3:uid="{5C657D4D-8A66-4157-8DB5-145B21A2134C}" name="disptabs" dataDxfId="37"/>
-    <tableColumn id="31" xr3:uid="{BB6C6479-DCFC-4184-88B3-AEDE3CAC59A3}" name="disporder" dataDxfId="36"/>
-    <tableColumn id="6" xr3:uid="{660D69F6-B312-40A1-9E4C-CFF43DBEC0B3}" name="source" dataDxfId="35"/>
-    <tableColumn id="2" xr3:uid="{172B3803-5494-4C90-B939-5C2F79872038}" name="sckey" dataDxfId="34"/>
-    <tableColumn id="14" xr3:uid="{3D01EE11-409F-43C6-990A-ABD3232293C0}" name="relkey" dataDxfId="33"/>
-    <tableColumn id="12" xr3:uid="{814C0F50-71A5-4E9D-9399-51983A27304D}" name="units" dataDxfId="32"/>
-    <tableColumn id="3" xr3:uid="{5F680C4B-D29A-4EFC-BE1D-FFAD04A6ECBF}" name="freq" dataDxfId="31"/>
-    <tableColumn id="10" xr3:uid="{ED9C9D35-83EF-4D33-B5A6-29714463F59D}" name="sa" dataDxfId="30"/>
-    <tableColumn id="4" xr3:uid="{4C279BEC-C29C-4B88-A87A-0A23F3DE4D9A}" name="st" dataDxfId="29"/>
-    <tableColumn id="13" xr3:uid="{4C82AECA-D40C-41E9-9170-45F127D67DD4}" name="d1" dataDxfId="28"/>
-    <tableColumn id="11" xr3:uid="{BCA31579-22E5-46AB-AC81-7237E8AE8CCD}" name="d2" dataDxfId="27"/>
-    <tableColumn id="16" xr3:uid="{5323D81D-334B-41E1-9C57-FB97D32790FE}" name="nc_dfm_input" dataDxfId="26"/>
-    <tableColumn id="17" xr3:uid="{136836AD-D381-4336-9040-09625567FE1C}" name="nc_method" dataDxfId="25"/>
-    <tableColumn id="29" xr3:uid="{76399FAE-BA60-4EB8-A76D-B35AF5C448A3}" name="initial_forecast" dataDxfId="24"/>
-    <tableColumn id="8" xr3:uid="{8D11F2D0-2DDA-4833-97A3-0AE2613B5941}" name="core_structural" dataDxfId="23"/>
-    <tableColumn id="18" xr3:uid="{5C5BF075-E0AE-47B3-8E6C-DA1E78BAA23F}" name="core_endog_type" dataDxfId="22"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{4AECC335-00AC-41E6-A3CA-F63691B92F69}" name="Table13279" displayName="Table13279" ref="A1:Q88" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
+  <autoFilter ref="A1:Q88" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
+  <tableColumns count="17">
+    <tableColumn id="1" xr3:uid="{CA6DE630-5CD5-428A-8439-1A504496E546}" name="varname" dataDxfId="16"/>
+    <tableColumn id="9" xr3:uid="{62B19A4C-5AC5-4FBE-B49F-BB64B9102385}" name="fullname" dataDxfId="15"/>
+    <tableColumn id="15" xr3:uid="{D22B03C4-4AE3-48C2-A598-07C9E704433D}" name="dispgroup" dataDxfId="14"/>
+    <tableColumn id="24" xr3:uid="{FDF2E866-66A2-44DE-B360-10560B9D2BFE}" name="disprank" dataDxfId="13"/>
+    <tableColumn id="25" xr3:uid="{5C657D4D-8A66-4157-8DB5-145B21A2134C}" name="disptabs" dataDxfId="12"/>
+    <tableColumn id="31" xr3:uid="{BB6C6479-DCFC-4184-88B3-AEDE3CAC59A3}" name="disporder" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{660D69F6-B312-40A1-9E4C-CFF43DBEC0B3}" name="source" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{172B3803-5494-4C90-B939-5C2F79872038}" name="sckey" dataDxfId="9"/>
+    <tableColumn id="14" xr3:uid="{3D01EE11-409F-43C6-990A-ABD3232293C0}" name="relkey" dataDxfId="8"/>
+    <tableColumn id="12" xr3:uid="{814C0F50-71A5-4E9D-9399-51983A27304D}" name="units" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{5F680C4B-D29A-4EFC-BE1D-FFAD04A6ECBF}" name="freq" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{ED9C9D35-83EF-4D33-B5A6-29714463F59D}" name="sa" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{4C279BEC-C29C-4B88-A87A-0A23F3DE4D9A}" name="st" dataDxfId="4"/>
+    <tableColumn id="13" xr3:uid="{4C82AECA-D40C-41E9-9170-45F127D67DD4}" name="d1" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{BCA31579-22E5-46AB-AC81-7237E8AE8CCD}" name="d2" dataDxfId="2"/>
+    <tableColumn id="16" xr3:uid="{5323D81D-334B-41E1-9C57-FB97D32790FE}" name="nc_dfm_input" dataDxfId="1"/>
+    <tableColumn id="17" xr3:uid="{136836AD-D381-4336-9040-09625567FE1C}" name="nc_method" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2319,16 +2156,16 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:W88"/>
+  <dimension ref="A1:T88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="S80" sqref="S80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="20.7109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="46.85546875" style="3" customWidth="1"/>
     <col min="3" max="3" width="11.140625" style="4" customWidth="1"/>
     <col min="4" max="6" width="9.5703125" style="4" customWidth="1"/>
     <col min="7" max="7" width="7.28515625" style="4" customWidth="1"/>
@@ -2338,15 +2175,14 @@
     <col min="11" max="11" width="9.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="6.85546875" style="4" customWidth="1"/>
     <col min="15" max="16" width="7.5703125" style="4" customWidth="1"/>
-    <col min="17" max="18" width="9.28515625" style="4" customWidth="1"/>
-    <col min="19" max="19" width="9.140625" style="4"/>
-    <col min="20" max="21" width="16.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="9.140625" style="3"/>
+    <col min="17" max="17" width="9.28515625" style="4" customWidth="1"/>
+    <col min="18" max="18" width="16.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2357,13 +2193,13 @@
         <v>196</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>392</v>
+        <v>382</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>394</v>
+        <v>384</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>98</v>
@@ -2372,7 +2208,7 @@
         <v>101</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>37</v>
@@ -2396,21 +2232,12 @@
         <v>252</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="R1" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="S1" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>381</v>
-      </c>
-      <c r="U1" s="3"/>
-      <c r="W1" s="3"/>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R1" s="3"/>
+      <c r="T1" s="3"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2436,10 +2263,10 @@
         <v>2</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>6</v>
@@ -2460,16 +2287,10 @@
       <c r="Q2" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="S2" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="T2" s="5" t="s">
-        <v>382</v>
-      </c>
-      <c r="U2" s="3"/>
-      <c r="W2" s="3"/>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R2" s="3"/>
+      <c r="T2" s="3"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>34</v>
       </c>
@@ -2495,10 +2316,10 @@
         <v>51</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>6</v>
@@ -2519,16 +2340,10 @@
       <c r="Q3" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="S3" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="T3" s="5" t="s">
-        <v>382</v>
-      </c>
-      <c r="U3" s="3"/>
-      <c r="W3" s="3"/>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R3" s="3"/>
+      <c r="T3" s="3"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>72</v>
       </c>
@@ -2554,10 +2369,10 @@
         <v>52</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>6</v>
@@ -2578,16 +2393,10 @@
       <c r="Q4" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="S4" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="T4" s="5" t="s">
-        <v>382</v>
-      </c>
-      <c r="U4" s="3"/>
-      <c r="W4" s="3"/>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R4" s="3"/>
+      <c r="T4" s="3"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>74</v>
       </c>
@@ -2613,10 +2422,10 @@
         <v>53</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="K5" s="4" t="s">
         <v>6</v>
@@ -2637,16 +2446,10 @@
       <c r="Q5" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="S5" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="T5" s="5" t="s">
-        <v>382</v>
-      </c>
-      <c r="U5" s="3"/>
-      <c r="W5" s="3"/>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R5" s="3"/>
+      <c r="T5" s="3"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>165</v>
       </c>
@@ -2672,10 +2475,10 @@
         <v>106</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="K6" s="4" t="s">
         <v>6</v>
@@ -2696,19 +2499,10 @@
       <c r="Q6" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="R6" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="S6" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="T6" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="U6" s="3"/>
-      <c r="W6" s="3"/>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R6" s="3"/>
+      <c r="T6" s="3"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>164</v>
       </c>
@@ -2734,10 +2528,10 @@
         <v>107</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="K7" s="4" t="s">
         <v>6</v>
@@ -2758,19 +2552,10 @@
       <c r="Q7" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="R7" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="S7" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="T7" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="U7" s="3"/>
-      <c r="W7" s="3"/>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R7" s="3"/>
+      <c r="T7" s="3"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>163</v>
       </c>
@@ -2796,10 +2581,10 @@
         <v>108</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="K8" s="4" t="s">
         <v>6</v>
@@ -2820,19 +2605,10 @@
       <c r="Q8" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="R8" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="S8" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="T8" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="U8" s="3"/>
-      <c r="W8" s="3"/>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R8" s="3"/>
+      <c r="T8" s="3"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>162</v>
       </c>
@@ -2858,10 +2634,10 @@
         <v>109</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="K9" s="4" t="s">
         <v>6</v>
@@ -2882,19 +2658,10 @@
       <c r="Q9" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="R9" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="S9" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="T9" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="U9" s="3"/>
-      <c r="W9" s="3"/>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R9" s="3"/>
+      <c r="T9" s="3"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>73</v>
       </c>
@@ -2920,10 +2687,10 @@
         <v>54</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="K10" s="4" t="s">
         <v>6</v>
@@ -2944,16 +2711,10 @@
       <c r="Q10" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="S10" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="T10" s="5" t="s">
-        <v>382</v>
-      </c>
-      <c r="U10" s="3"/>
-      <c r="W10" s="3"/>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R10" s="3"/>
+      <c r="T10" s="3"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>110</v>
       </c>
@@ -2979,10 +2740,10 @@
         <v>55</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="K11" s="4" t="s">
         <v>6</v>
@@ -3003,19 +2764,10 @@
       <c r="Q11" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="R11" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="S11" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="T11" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="U11" s="3"/>
-      <c r="W11" s="3"/>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R11" s="3"/>
+      <c r="T11" s="3"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>111</v>
       </c>
@@ -3041,10 +2793,10 @@
         <v>114</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="K12" s="4" t="s">
         <v>6</v>
@@ -3065,19 +2817,10 @@
       <c r="Q12" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="R12" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="S12" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="T12" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="U12" s="3"/>
-      <c r="W12" s="3"/>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R12" s="3"/>
+      <c r="T12" s="3"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>112</v>
       </c>
@@ -3103,10 +2846,10 @@
         <v>115</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="K13" s="4" t="s">
         <v>6</v>
@@ -3127,19 +2870,10 @@
       <c r="Q13" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="R13" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="S13" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="T13" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="U13" s="3"/>
-      <c r="W13" s="3"/>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R13" s="3"/>
+      <c r="T13" s="3"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>113</v>
       </c>
@@ -3165,10 +2899,10 @@
         <v>116</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="K14" s="4" t="s">
         <v>6</v>
@@ -3189,19 +2923,10 @@
       <c r="Q14" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="R14" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="S14" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="T14" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="U14" s="3"/>
-      <c r="W14" s="3"/>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R14" s="3"/>
+      <c r="T14" s="3"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>75</v>
       </c>
@@ -3227,10 +2952,10 @@
         <v>56</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="K15" s="4" t="s">
         <v>6</v>
@@ -3251,16 +2976,10 @@
       <c r="Q15" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="S15" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="T15" s="5" t="s">
-        <v>382</v>
-      </c>
-      <c r="U15" s="3"/>
-      <c r="W15" s="3"/>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R15" s="3"/>
+      <c r="T15" s="3"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>76</v>
       </c>
@@ -3286,10 +3005,10 @@
         <v>57</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="K16" s="4" t="s">
         <v>6</v>
@@ -3310,19 +3029,10 @@
       <c r="Q16" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="R16" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="S16" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="T16" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="U16" s="3"/>
-      <c r="W16" s="3"/>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R16" s="3"/>
+      <c r="T16" s="3"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>80</v>
       </c>
@@ -3348,10 +3058,10 @@
         <v>58</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="K17" s="4" t="s">
         <v>6</v>
@@ -3372,19 +3082,10 @@
       <c r="Q17" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="R17" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="S17" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="T17" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="U17" s="3"/>
-      <c r="W17" s="3"/>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R17" s="3"/>
+      <c r="T17" s="3"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>119</v>
       </c>
@@ -3410,10 +3111,10 @@
         <v>59</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="K18" s="4" t="s">
         <v>6</v>
@@ -3434,19 +3135,10 @@
       <c r="Q18" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="R18" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="S18" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="T18" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="U18" s="3"/>
-      <c r="W18" s="3"/>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R18" s="3"/>
+      <c r="T18" s="3"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>82</v>
       </c>
@@ -3472,10 +3164,10 @@
         <v>60</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="K19" s="4" t="s">
         <v>6</v>
@@ -3496,19 +3188,10 @@
       <c r="Q19" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="R19" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="S19" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="T19" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="U19" s="3"/>
-      <c r="W19" s="3"/>
-    </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R19" s="3"/>
+      <c r="T19" s="3"/>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>77</v>
       </c>
@@ -3534,10 +3217,10 @@
         <v>61</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="K20" s="4" t="s">
         <v>6</v>
@@ -3558,19 +3241,10 @@
       <c r="Q20" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="R20" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="S20" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="T20" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="U20" s="3"/>
-      <c r="W20" s="3"/>
-    </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R20" s="3"/>
+      <c r="T20" s="3"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>79</v>
       </c>
@@ -3596,10 +3270,10 @@
         <v>62</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="K21" s="4" t="s">
         <v>6</v>
@@ -3620,19 +3294,10 @@
       <c r="Q21" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="R21" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="S21" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="T21" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="U21" s="3"/>
-      <c r="W21" s="3"/>
-    </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R21" s="3"/>
+      <c r="T21" s="3"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>78</v>
       </c>
@@ -3658,10 +3323,10 @@
         <v>63</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="K22" s="4" t="s">
         <v>6</v>
@@ -3682,19 +3347,10 @@
       <c r="Q22" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="R22" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="S22" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="T22" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="U22" s="3"/>
-      <c r="W22" s="3"/>
-    </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R22" s="3"/>
+      <c r="T22" s="3"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>83</v>
       </c>
@@ -3720,10 +3376,10 @@
         <v>64</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="K23" s="4" t="s">
         <v>6</v>
@@ -3744,19 +3400,10 @@
       <c r="Q23" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="R23" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="S23" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="T23" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="U23" s="3"/>
-      <c r="W23" s="3"/>
-    </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R23" s="3"/>
+      <c r="T23" s="3"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>48</v>
       </c>
@@ -3782,10 +3429,10 @@
         <v>47</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="K24" s="4" t="s">
         <v>6</v>
@@ -3806,16 +3453,10 @@
       <c r="Q24" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="S24" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="T24" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="U24" s="3"/>
-      <c r="W24" s="3"/>
-    </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R24" s="3"/>
+      <c r="T24" s="3"/>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>118</v>
       </c>
@@ -3841,10 +3482,10 @@
         <v>65</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="K25" s="4" t="s">
         <v>6</v>
@@ -3865,16 +3506,10 @@
       <c r="Q25" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="S25" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="T25" s="5" t="s">
-        <v>382</v>
-      </c>
-      <c r="U25" s="3"/>
-      <c r="W25" s="3"/>
-    </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R25" s="3"/>
+      <c r="T25" s="3"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>120</v>
       </c>
@@ -3900,10 +3535,10 @@
         <v>126</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="K26" s="4" t="s">
         <v>6</v>
@@ -3924,19 +3559,10 @@
       <c r="Q26" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="R26" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="S26" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="T26" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="U26" s="3"/>
-      <c r="W26" s="3"/>
-    </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R26" s="3"/>
+      <c r="T26" s="3"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>121</v>
       </c>
@@ -3962,10 +3588,10 @@
         <v>127</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="K27" s="4" t="s">
         <v>6</v>
@@ -3986,19 +3612,10 @@
       <c r="Q27" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="R27" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="S27" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="T27" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="U27" s="3"/>
-      <c r="W27" s="3"/>
-    </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R27" s="3"/>
+      <c r="T27" s="3"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>122</v>
       </c>
@@ -4024,10 +3641,10 @@
         <v>128</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="K28" s="4" t="s">
         <v>6</v>
@@ -4048,19 +3665,10 @@
       <c r="Q28" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="R28" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="S28" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="T28" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="U28" s="3"/>
-      <c r="W28" s="3"/>
-    </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R28" s="3"/>
+      <c r="T28" s="3"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>85</v>
       </c>
@@ -4086,10 +3694,10 @@
         <v>66</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="K29" s="4" t="s">
         <v>6</v>
@@ -4110,19 +3718,10 @@
       <c r="Q29" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="R29" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="S29" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="T29" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="U29" s="3"/>
-      <c r="W29" s="3"/>
-    </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R29" s="3"/>
+      <c r="T29" s="3"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>81</v>
       </c>
@@ -4148,10 +3747,10 @@
         <v>67</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="K30" s="4" t="s">
         <v>6</v>
@@ -4172,14 +3771,10 @@
       <c r="Q30" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="S30" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="T30" s="5"/>
-      <c r="U30" s="3"/>
-      <c r="W30" s="3"/>
-    </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R30" s="3"/>
+      <c r="T30" s="3"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>89</v>
       </c>
@@ -4205,10 +3800,10 @@
         <v>68</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="K31" s="4" t="s">
         <v>6</v>
@@ -4229,14 +3824,10 @@
       <c r="Q31" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="S31" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="T31" s="5"/>
-      <c r="U31" s="3"/>
-      <c r="W31" s="3"/>
-    </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R31" s="3"/>
+      <c r="T31" s="3"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>91</v>
       </c>
@@ -4262,10 +3853,10 @@
         <v>104</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="K32" s="4" t="s">
         <v>6</v>
@@ -4286,16 +3877,10 @@
       <c r="Q32" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="S32" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="T32" s="5" t="s">
-        <v>382</v>
-      </c>
-      <c r="U32" s="3"/>
-      <c r="W32" s="3"/>
-    </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R32" s="3"/>
+      <c r="T32" s="3"/>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>129</v>
       </c>
@@ -4321,10 +3906,10 @@
         <v>133</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="K33" s="4" t="s">
         <v>6</v>
@@ -4345,19 +3930,10 @@
       <c r="Q33" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="R33" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="S33" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="T33" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="U33" s="3"/>
-      <c r="W33" s="3"/>
-    </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R33" s="3"/>
+      <c r="T33" s="3"/>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>130</v>
       </c>
@@ -4383,10 +3959,10 @@
         <v>134</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="K34" s="4" t="s">
         <v>6</v>
@@ -4407,19 +3983,10 @@
       <c r="Q34" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="R34" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="S34" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="T34" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="U34" s="3"/>
-      <c r="W34" s="3"/>
-    </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R34" s="3"/>
+      <c r="T34" s="3"/>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>92</v>
       </c>
@@ -4445,10 +4012,10 @@
         <v>103</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="K35" s="4" t="s">
         <v>6</v>
@@ -4469,16 +4036,10 @@
       <c r="Q35" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="S35" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="T35" s="5" t="s">
-        <v>382</v>
-      </c>
-      <c r="U35" s="3"/>
-      <c r="W35" s="3"/>
-    </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R35" s="3"/>
+      <c r="T35" s="3"/>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>131</v>
       </c>
@@ -4504,10 +4065,10 @@
         <v>135</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="K36" s="4" t="s">
         <v>6</v>
@@ -4528,19 +4089,10 @@
       <c r="Q36" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="R36" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="S36" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="T36" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="U36" s="3"/>
-      <c r="W36" s="3"/>
-    </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R36" s="3"/>
+      <c r="T36" s="3"/>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>132</v>
       </c>
@@ -4566,10 +4118,10 @@
         <v>136</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="K37" s="4" t="s">
         <v>6</v>
@@ -4590,19 +4142,10 @@
       <c r="Q37" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="R37" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="S37" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="T37" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="U37" s="3"/>
-      <c r="W37" s="3"/>
-    </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R37" s="3"/>
+      <c r="T37" s="3"/>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>93</v>
       </c>
@@ -4628,10 +4171,10 @@
         <v>69</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="K38" s="4" t="s">
         <v>6</v>
@@ -4652,16 +4195,10 @@
       <c r="Q38" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="S38" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="T38" s="5" t="s">
-        <v>382</v>
-      </c>
-      <c r="U38" s="3"/>
-      <c r="W38" s="3"/>
-    </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R38" s="3"/>
+      <c r="T38" s="3"/>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>94</v>
       </c>
@@ -4687,10 +4224,10 @@
         <v>70</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="K39" s="4" t="s">
         <v>6</v>
@@ -4711,19 +4248,10 @@
       <c r="Q39" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="R39" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="S39" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="T39" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="U39" s="3"/>
-      <c r="W39" s="3"/>
-    </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R39" s="3"/>
+      <c r="T39" s="3"/>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>95</v>
       </c>
@@ -4749,10 +4277,10 @@
         <v>71</v>
       </c>
       <c r="I40" s="4" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="K40" s="4" t="s">
         <v>6</v>
@@ -4773,19 +4301,10 @@
       <c r="Q40" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="R40" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="S40" s="5" t="s">
-        <v>384</v>
-      </c>
-      <c r="T40" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="U40" s="3"/>
-      <c r="W40" s="3"/>
-    </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R40" s="3"/>
+      <c r="T40" s="3"/>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>117</v>
       </c>
@@ -4799,10 +4318,10 @@
         <v>45</v>
       </c>
       <c r="I41" s="4" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="K41" s="4" t="s">
         <v>7</v>
@@ -4825,14 +4344,10 @@
       <c r="Q41" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="S41" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="T41" s="5"/>
-      <c r="U41" s="3"/>
-      <c r="W41" s="3"/>
-    </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R41" s="3"/>
+      <c r="T41" s="3"/>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>139</v>
       </c>
@@ -4846,10 +4361,10 @@
         <v>140</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="K42" s="4" t="s">
         <v>7</v>
@@ -4872,14 +4387,10 @@
       <c r="Q42" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="S42" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="T42" s="5"/>
-      <c r="U42" s="3"/>
-      <c r="W42" s="3"/>
-    </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R42" s="3"/>
+      <c r="T42" s="3"/>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>144</v>
       </c>
@@ -4893,10 +4404,10 @@
         <v>150</v>
       </c>
       <c r="I43" s="4" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="K43" s="4" t="s">
         <v>7</v>
@@ -4919,14 +4430,10 @@
       <c r="Q43" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="S43" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="T43" s="5"/>
-      <c r="U43" s="3"/>
-      <c r="W43" s="3"/>
-    </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R43" s="3"/>
+      <c r="T43" s="3"/>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>146</v>
       </c>
@@ -4940,10 +4447,10 @@
         <v>149</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="K44" s="4" t="s">
         <v>7</v>
@@ -4966,19 +4473,15 @@
       <c r="Q44" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="S44" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="T44" s="5"/>
-      <c r="U44" s="3"/>
-      <c r="W44" s="3"/>
-    </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R44" s="3"/>
+      <c r="T44" s="3"/>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>387</v>
+        <v>377</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>220</v>
@@ -4999,7 +4502,7 @@
         <v>9</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="J45" s="4" t="s">
         <v>41</v>
@@ -5025,22 +4528,15 @@
       <c r="Q45" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="R45" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="S45" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="T45" s="5"/>
-      <c r="U45" s="3"/>
-      <c r="W45" s="3"/>
-    </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R45" s="3"/>
+      <c r="T45" s="3"/>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>388</v>
+        <v>378</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>220</v>
@@ -5058,10 +4554,10 @@
         <v>99</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="J46" s="4" t="s">
         <v>41</v>
@@ -5087,17 +4583,10 @@
       <c r="Q46" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="R46" s="5"/>
-      <c r="S46" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="T46" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="U46" s="3"/>
-      <c r="W46" s="3"/>
-    </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R46" s="3"/>
+      <c r="T46" s="3"/>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>208</v>
       </c>
@@ -5123,7 +4612,7 @@
         <v>210</v>
       </c>
       <c r="I47" s="4" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="J47" s="4" t="s">
         <v>222</v>
@@ -5149,16 +4638,10 @@
       <c r="Q47" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="S47" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="T47" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="U47" s="3"/>
-      <c r="W47" s="3"/>
-    </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R47" s="3"/>
+      <c r="T47" s="3"/>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>218</v>
       </c>
@@ -5184,7 +4667,7 @@
         <v>221</v>
       </c>
       <c r="I48" s="4" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="J48" s="4" t="s">
         <v>222</v>
@@ -5210,16 +4693,10 @@
       <c r="Q48" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="S48" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="T48" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="U48" s="3"/>
-      <c r="W48" s="3"/>
-    </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R48" s="3"/>
+      <c r="T48" s="3"/>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>225</v>
       </c>
@@ -5245,7 +4722,7 @@
         <v>227</v>
       </c>
       <c r="I49" s="4" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="J49" s="4" t="s">
         <v>222</v>
@@ -5271,21 +4748,15 @@
       <c r="Q49" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="S49" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="T49" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="U49" s="3"/>
-      <c r="W49" s="3"/>
-    </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R49" s="3"/>
+      <c r="T49" s="3"/>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>418</v>
+        <v>408</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>419</v>
+        <v>409</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>220</v>
@@ -5303,10 +4774,10 @@
         <v>99</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>420</v>
+        <v>410</v>
       </c>
       <c r="I50" s="4" t="s">
-        <v>421</v>
+        <v>411</v>
       </c>
       <c r="J50" s="4" t="s">
         <v>41</v>
@@ -5332,17 +4803,10 @@
       <c r="Q50" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="R50" s="5"/>
-      <c r="S50" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="T50" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="U50" s="3"/>
-      <c r="W50" s="3"/>
-    </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R50" s="3"/>
+      <c r="T50" s="3"/>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>223</v>
       </c>
@@ -5356,10 +4820,10 @@
         <v>224</v>
       </c>
       <c r="I51" s="4" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>401</v>
+        <v>391</v>
       </c>
       <c r="K51" s="4" t="s">
         <v>7</v>
@@ -5382,14 +4846,10 @@
       <c r="Q51" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="S51" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="T51" s="5"/>
-      <c r="U51" s="3"/>
-      <c r="W51" s="3"/>
-    </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R51" s="3"/>
+      <c r="T51" s="3"/>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>215</v>
       </c>
@@ -5403,10 +4863,10 @@
         <v>217</v>
       </c>
       <c r="I52" s="4" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>401</v>
+        <v>391</v>
       </c>
       <c r="K52" s="4" t="s">
         <v>7</v>
@@ -5429,14 +4889,10 @@
       <c r="Q52" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="S52" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="T52" s="5"/>
-      <c r="U52" s="3"/>
-      <c r="W52" s="3"/>
-    </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R52" s="3"/>
+      <c r="T52" s="3"/>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>11</v>
       </c>
@@ -5444,7 +4900,7 @@
         <v>25</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>397</v>
+        <v>387</v>
       </c>
       <c r="D53" s="4">
         <v>2</v>
@@ -5462,10 +4918,10 @@
         <v>10</v>
       </c>
       <c r="I53" s="4" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="J53" s="4" t="s">
-        <v>405</v>
+        <v>395</v>
       </c>
       <c r="K53" s="4" t="s">
         <v>7</v>
@@ -5488,16 +4944,10 @@
       <c r="Q53" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="S53" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="T53" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="U53" s="3"/>
-      <c r="W53" s="3"/>
-    </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R53" s="3"/>
+      <c r="T53" s="3"/>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>211</v>
       </c>
@@ -5505,7 +4955,7 @@
         <v>212</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>396</v>
+        <v>386</v>
       </c>
       <c r="D54" s="4">
         <v>3</v>
@@ -5523,7 +4973,7 @@
         <v>214</v>
       </c>
       <c r="I54" s="4" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="J54" s="4" t="s">
         <v>222</v>
@@ -5549,24 +4999,18 @@
       <c r="Q54" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="S54" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="T54" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="U54" s="3"/>
-      <c r="W54" s="3"/>
-    </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R54" s="3"/>
+      <c r="T54" s="3"/>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>229</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>396</v>
+        <v>386</v>
       </c>
       <c r="D55" s="4">
         <v>3</v>
@@ -5584,7 +5028,7 @@
         <v>230</v>
       </c>
       <c r="I55" s="4" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="J55" s="4" t="s">
         <v>222</v>
@@ -5610,24 +5054,18 @@
       <c r="Q55" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="S55" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="T55" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="U55" s="3"/>
-      <c r="W55" s="3"/>
-    </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R55" s="3"/>
+      <c r="T55" s="3"/>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>423</v>
+        <v>413</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>424</v>
+        <v>414</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>396</v>
+        <v>386</v>
       </c>
       <c r="D56" s="4">
         <v>3</v>
@@ -5642,10 +5080,10 @@
         <v>99</v>
       </c>
       <c r="H56" s="4" t="s">
-        <v>425</v>
+        <v>415</v>
       </c>
       <c r="I56" s="4" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="J56" s="4" t="s">
         <v>222</v>
@@ -5671,21 +5109,18 @@
       <c r="Q56" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="R56" s="5"/>
-      <c r="S56" s="5"/>
-      <c r="T56" s="5"/>
-      <c r="U56" s="3"/>
-      <c r="W56" s="3"/>
-    </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R56" s="3"/>
+      <c r="T56" s="3"/>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>433</v>
+        <v>423</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>434</v>
+        <v>424</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>396</v>
+        <v>386</v>
       </c>
       <c r="D57" s="4">
         <v>1</v>
@@ -5700,13 +5135,13 @@
         <v>99</v>
       </c>
       <c r="H57" s="4" t="s">
-        <v>435</v>
+        <v>425</v>
       </c>
       <c r="I57" s="4" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="J57" s="4" t="s">
-        <v>436</v>
+        <v>426</v>
       </c>
       <c r="K57" s="4" t="s">
         <v>7</v>
@@ -5715,7 +5150,7 @@
         <v>250</v>
       </c>
       <c r="M57" s="4" t="s">
-        <v>385</v>
+        <v>375</v>
       </c>
       <c r="N57" s="4" t="s">
         <v>4</v>
@@ -5729,17 +5164,10 @@
       <c r="Q57" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="R57" s="5"/>
-      <c r="S57" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="T57" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="U57" s="3"/>
-      <c r="W57" s="3"/>
-    </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R57" s="3"/>
+      <c r="T57" s="3"/>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>231</v>
       </c>
@@ -5747,7 +5175,7 @@
         <v>232</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>398</v>
+        <v>388</v>
       </c>
       <c r="D58" s="4">
         <v>2</v>
@@ -5765,10 +5193,10 @@
         <v>233</v>
       </c>
       <c r="I58" s="4" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="J58" s="4" t="s">
-        <v>404</v>
+        <v>394</v>
       </c>
       <c r="K58" s="4" t="s">
         <v>241</v>
@@ -5791,24 +5219,18 @@
       <c r="Q58" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="S58" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="T58" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="U58" s="3"/>
-      <c r="W58" s="3"/>
-    </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R58" s="3"/>
+      <c r="T58" s="3"/>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="C59" s="4" t="s">
         <v>376</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>386</v>
       </c>
       <c r="D59" s="4">
         <v>2</v>
@@ -5823,13 +5245,13 @@
         <v>99</v>
       </c>
       <c r="H59" s="4" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="I59" s="4" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>400</v>
+        <v>390</v>
       </c>
       <c r="K59" s="4" t="s">
         <v>247</v>
@@ -5852,24 +5274,18 @@
       <c r="Q59" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="S59" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="T59" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="U59" s="3"/>
-      <c r="W59" s="3"/>
-    </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R59" s="3"/>
+      <c r="T59" s="3"/>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>386</v>
+        <v>376</v>
       </c>
       <c r="D60" s="4">
         <v>2</v>
@@ -5884,13 +5300,13 @@
         <v>99</v>
       </c>
       <c r="H60" s="4" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="I60" s="4" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="J60" s="4" t="s">
-        <v>400</v>
+        <v>390</v>
       </c>
       <c r="K60" s="4" t="s">
         <v>247</v>
@@ -5913,24 +5329,18 @@
       <c r="Q60" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="S60" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="T60" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="U60" s="3"/>
-      <c r="W60" s="3"/>
-    </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R60" s="3"/>
+      <c r="T60" s="3"/>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>386</v>
+        <v>376</v>
       </c>
       <c r="D61" s="4">
         <v>2</v>
@@ -5948,10 +5358,10 @@
         <v>16</v>
       </c>
       <c r="I61" s="4" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="J61" s="4" t="s">
-        <v>400</v>
+        <v>390</v>
       </c>
       <c r="K61" s="4" t="s">
         <v>247</v>
@@ -5974,16 +5384,10 @@
       <c r="Q61" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="S61" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="T61" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="U61" s="3"/>
-      <c r="W61" s="3"/>
-    </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R61" s="3"/>
+      <c r="T61" s="3"/>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>17</v>
       </c>
@@ -5994,10 +5398,10 @@
         <v>99</v>
       </c>
       <c r="H62" s="4" t="s">
-        <v>413</v>
+        <v>403</v>
       </c>
       <c r="I62" s="4" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="J62" s="4" t="s">
         <v>41</v>
@@ -6023,14 +5427,10 @@
       <c r="Q62" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="S62" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="T62" s="5"/>
-      <c r="U62" s="3"/>
-      <c r="W62" s="3"/>
-    </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R62" s="3"/>
+      <c r="T62" s="3"/>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>18</v>
       </c>
@@ -6038,7 +5438,7 @@
         <v>28</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>393</v>
+        <v>383</v>
       </c>
       <c r="D63" s="4">
         <v>1</v>
@@ -6053,10 +5453,10 @@
         <v>166</v>
       </c>
       <c r="H63" s="4" t="s">
-        <v>417</v>
+        <v>407</v>
       </c>
       <c r="I63" s="4" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="J63" s="4" t="s">
         <v>41</v>
@@ -6068,7 +5468,7 @@
         <v>250</v>
       </c>
       <c r="M63" s="4" t="s">
-        <v>385</v>
+        <v>375</v>
       </c>
       <c r="N63" s="4" t="s">
         <v>4</v>
@@ -6082,16 +5482,10 @@
       <c r="Q63" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="S63" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="T63" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="U63" s="3"/>
-      <c r="W63" s="3"/>
-    </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R63" s="3"/>
+      <c r="T63" s="3"/>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>19</v>
       </c>
@@ -6099,7 +5493,7 @@
         <v>39</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>397</v>
+        <v>387</v>
       </c>
       <c r="D64" s="4">
         <v>1</v>
@@ -6114,13 +5508,13 @@
         <v>99</v>
       </c>
       <c r="H64" s="4" t="s">
-        <v>395</v>
+        <v>385</v>
       </c>
       <c r="I64" s="4" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>401</v>
+        <v>391</v>
       </c>
       <c r="K64" s="4" t="s">
         <v>7</v>
@@ -6143,16 +5537,10 @@
       <c r="Q64" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="S64" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="T64" s="5" t="s">
-        <v>382</v>
-      </c>
-      <c r="U64" s="3"/>
-      <c r="W64" s="3"/>
-    </row>
-    <row r="65" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R64" s="3"/>
+      <c r="T64" s="3"/>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>20</v>
       </c>
@@ -6166,7 +5554,7 @@
         <v>21</v>
       </c>
       <c r="I65" s="4" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="J65" s="4" t="s">
         <v>41</v>
@@ -6192,14 +5580,10 @@
       <c r="Q65" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="S65" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="T65" s="5"/>
-      <c r="U65" s="3"/>
-      <c r="W65" s="3"/>
-    </row>
-    <row r="66" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R65" s="3"/>
+      <c r="T65" s="3"/>
+    </row>
+    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>29</v>
       </c>
@@ -6213,7 +5597,7 @@
         <v>31</v>
       </c>
       <c r="I66" s="4" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="J66" s="4" t="s">
         <v>41</v>
@@ -6239,14 +5623,10 @@
       <c r="Q66" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="S66" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="T66" s="5"/>
-      <c r="U66" s="3"/>
-      <c r="W66" s="3"/>
-    </row>
-    <row r="67" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R66" s="3"/>
+      <c r="T66" s="3"/>
+    </row>
+    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>151</v>
       </c>
@@ -6260,7 +5640,7 @@
         <v>33</v>
       </c>
       <c r="I67" s="4" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="J67" s="4" t="s">
         <v>41</v>
@@ -6286,31 +5666,27 @@
       <c r="Q67" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="S67" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="T67" s="5"/>
-      <c r="U67" s="3"/>
-      <c r="W67" s="3"/>
-    </row>
-    <row r="68" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R67" s="3"/>
+      <c r="T67" s="3"/>
+    </row>
+    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>426</v>
+        <v>416</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>427</v>
+        <v>417</v>
       </c>
       <c r="G68" s="4" t="s">
         <v>99</v>
       </c>
       <c r="H68" s="4" t="s">
-        <v>428</v>
+        <v>418</v>
       </c>
       <c r="I68" s="4" t="s">
-        <v>429</v>
+        <v>419</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>432</v>
+        <v>422</v>
       </c>
       <c r="K68" s="4" t="s">
         <v>7</v>
@@ -6333,15 +5709,10 @@
       <c r="Q68" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="R68" s="5"/>
-      <c r="S68" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="T68" s="5"/>
-      <c r="U68" s="3"/>
-      <c r="W68" s="3"/>
-    </row>
-    <row r="69" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R68" s="3"/>
+      <c r="T68" s="3"/>
+    </row>
+    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>42</v>
       </c>
@@ -6355,10 +5726,10 @@
         <v>43</v>
       </c>
       <c r="I69" s="4" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="J69" s="4" t="s">
-        <v>402</v>
+        <v>392</v>
       </c>
       <c r="K69" s="4" t="s">
         <v>7</v>
@@ -6381,14 +5752,10 @@
       <c r="Q69" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="S69" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="T69" s="5"/>
-      <c r="U69" s="3"/>
-      <c r="W69" s="3"/>
-    </row>
-    <row r="70" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R69" s="3"/>
+      <c r="T69" s="3"/>
+    </row>
+    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>152</v>
       </c>
@@ -6396,7 +5763,7 @@
         <v>153</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>386</v>
+        <v>376</v>
       </c>
       <c r="D70" s="4">
         <v>1</v>
@@ -6414,7 +5781,7 @@
         <v>158</v>
       </c>
       <c r="I70" s="4" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="J70" s="4" t="s">
         <v>38</v>
@@ -6438,16 +5805,10 @@
       <c r="Q70" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="S70" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="T70" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="U70" s="3"/>
-      <c r="W70" s="3"/>
-    </row>
-    <row r="71" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R70" s="3"/>
+      <c r="T70" s="3"/>
+    </row>
+    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>154</v>
       </c>
@@ -6455,7 +5816,7 @@
         <v>155</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>386</v>
+        <v>376</v>
       </c>
       <c r="D71" s="4">
         <v>1</v>
@@ -6473,7 +5834,7 @@
         <v>159</v>
       </c>
       <c r="I71" s="4" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="J71" s="4" t="s">
         <v>38</v>
@@ -6497,16 +5858,10 @@
       <c r="Q71" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="S71" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="T71" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="U71" s="3"/>
-      <c r="W71" s="3"/>
-    </row>
-    <row r="72" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R71" s="3"/>
+      <c r="T71" s="3"/>
+    </row>
+    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>156</v>
       </c>
@@ -6514,7 +5869,7 @@
         <v>157</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>386</v>
+        <v>376</v>
       </c>
       <c r="D72" s="4">
         <v>1</v>
@@ -6532,7 +5887,7 @@
         <v>160</v>
       </c>
       <c r="I72" s="4" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="J72" s="4" t="s">
         <v>38</v>
@@ -6556,30 +5911,24 @@
       <c r="Q72" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="S72" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="T72" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="U72" s="3"/>
-      <c r="W72" s="3"/>
-    </row>
-    <row r="73" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R72" s="3"/>
+      <c r="T72" s="3"/>
+    </row>
+    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>202</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
       <c r="G73" s="4" t="s">
         <v>99</v>
       </c>
       <c r="H73" s="4" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="I73" s="4" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="J73" s="4" t="s">
         <v>41</v>
@@ -6605,14 +5954,10 @@
       <c r="Q73" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="S73" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="T73" s="5"/>
-      <c r="U73" s="3"/>
-      <c r="W73" s="3"/>
-    </row>
-    <row r="74" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R73" s="3"/>
+      <c r="T73" s="3"/>
+    </row>
+    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>203</v>
       </c>
@@ -6626,7 +5971,7 @@
         <v>161</v>
       </c>
       <c r="I74" s="4" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="J74" s="4" t="s">
         <v>41</v>
@@ -6652,14 +5997,10 @@
       <c r="Q74" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="S74" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="T74" s="5"/>
-      <c r="U74" s="3"/>
-      <c r="W74" s="3"/>
-    </row>
-    <row r="75" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R74" s="3"/>
+      <c r="T74" s="3"/>
+    </row>
+    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>204</v>
       </c>
@@ -6673,7 +6014,7 @@
         <v>206</v>
       </c>
       <c r="I75" s="4" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="J75" s="4" t="s">
         <v>41</v>
@@ -6699,14 +6040,10 @@
       <c r="Q75" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="S75" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="T75" s="5"/>
-      <c r="U75" s="3"/>
-      <c r="W75" s="3"/>
-    </row>
-    <row r="76" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R75" s="3"/>
+      <c r="T75" s="3"/>
+    </row>
+    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>234</v>
       </c>
@@ -6720,7 +6057,7 @@
         <v>236</v>
       </c>
       <c r="I76" s="4" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="J76" s="4" t="s">
         <v>38</v>
@@ -6746,14 +6083,10 @@
       <c r="Q76" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="S76" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="T76" s="5"/>
-      <c r="U76" s="3"/>
-      <c r="W76" s="3"/>
-    </row>
-    <row r="77" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R76" s="3"/>
+      <c r="T76" s="3"/>
+    </row>
+    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>237</v>
       </c>
@@ -6767,7 +6100,7 @@
         <v>239</v>
       </c>
       <c r="I77" s="4" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="J77" s="4" t="s">
         <v>38</v>
@@ -6793,14 +6126,10 @@
       <c r="Q77" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="S77" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="T77" s="5"/>
-      <c r="U77" s="3"/>
-      <c r="W77" s="3"/>
-    </row>
-    <row r="78" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R77" s="3"/>
+      <c r="T77" s="3"/>
+    </row>
+    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>242</v>
       </c>
@@ -6814,7 +6143,7 @@
         <v>244</v>
       </c>
       <c r="I78" s="4" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="J78" s="4" t="s">
         <v>41</v>
@@ -6840,14 +6169,10 @@
       <c r="Q78" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="S78" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="T78" s="5"/>
-      <c r="U78" s="3"/>
-      <c r="W78" s="3"/>
-    </row>
-    <row r="79" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R78" s="3"/>
+      <c r="T78" s="3"/>
+    </row>
+    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>245</v>
       </c>
@@ -6871,7 +6196,7 @@
       </c>
       <c r="H79" s="4"/>
       <c r="I79" s="4" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="J79" s="4" t="s">
         <v>38</v>
@@ -6897,17 +6222,10 @@
       <c r="Q79" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="R79" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="S79" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="T79" s="5"/>
-      <c r="U79" s="3"/>
-      <c r="W79" s="3"/>
-    </row>
-    <row r="80" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R79" s="3"/>
+      <c r="T79" s="3"/>
+    </row>
+    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>14</v>
       </c>
@@ -6915,7 +6233,7 @@
         <v>26</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>398</v>
+        <v>388</v>
       </c>
       <c r="D80" s="4">
         <v>1</v>
@@ -6933,7 +6251,7 @@
         <v>200</v>
       </c>
       <c r="I80" s="4" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="J80" s="4" t="s">
         <v>41</v>
@@ -6959,17 +6277,10 @@
       <c r="Q80" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="R80" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="S80" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="T80" s="5"/>
-      <c r="U80" s="3"/>
-      <c r="W80" s="3"/>
-    </row>
-    <row r="81" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R80" s="3"/>
+      <c r="T80" s="3"/>
+    </row>
+    <row r="81" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>15</v>
       </c>
@@ -6977,7 +6288,7 @@
         <v>24</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>398</v>
+        <v>388</v>
       </c>
       <c r="D81" s="4">
         <v>2</v>
@@ -6995,7 +6306,7 @@
         <v>201</v>
       </c>
       <c r="I81" s="4" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="J81" s="4" t="s">
         <v>41</v>
@@ -7021,24 +6332,18 @@
       <c r="Q81" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="S81" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="T81" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="U81" s="3"/>
-      <c r="W81" s="3"/>
-    </row>
-    <row r="82" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R81" s="3"/>
+      <c r="T81" s="3"/>
+    </row>
+    <row r="82" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>398</v>
+        <v>388</v>
       </c>
       <c r="D82" s="4">
         <v>2</v>
@@ -7053,10 +6358,10 @@
         <v>166</v>
       </c>
       <c r="H82" s="4" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="I82" s="4" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="J82" s="4" t="s">
         <v>41</v>
@@ -7082,24 +6387,18 @@
       <c r="Q82" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="S82" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="T82" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="U82" s="3"/>
-      <c r="W82" s="3"/>
-    </row>
-    <row r="83" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R82" s="3"/>
+      <c r="T82" s="3"/>
+    </row>
+    <row r="83" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="B83" s="3" t="s">
         <v>365</v>
       </c>
-      <c r="B83" s="3" t="s">
-        <v>370</v>
-      </c>
       <c r="C83" s="4" t="s">
-        <v>398</v>
+        <v>388</v>
       </c>
       <c r="D83" s="4">
         <v>2</v>
@@ -7114,10 +6413,10 @@
         <v>166</v>
       </c>
       <c r="H83" s="4" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="I83" s="4" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="J83" s="4" t="s">
         <v>41</v>
@@ -7143,30 +6442,24 @@
       <c r="Q83" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="S83" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="T83" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="U83" s="3"/>
-      <c r="W83" s="3"/>
-    </row>
-    <row r="84" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R83" s="3"/>
+      <c r="T83" s="3"/>
+    </row>
+    <row r="84" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="G84" s="4" t="s">
         <v>166</v>
       </c>
       <c r="H84" s="4" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="I84" s="4" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="J84" s="4" t="s">
         <v>41</v>
@@ -7192,14 +6485,10 @@
       <c r="Q84" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="S84" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="T84" s="5"/>
-      <c r="U84" s="3"/>
-      <c r="W84" s="3"/>
-    </row>
-    <row r="85" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R84" s="3"/>
+      <c r="T84" s="3"/>
+    </row>
+    <row r="85" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>137</v>
       </c>
@@ -7213,10 +6502,10 @@
         <v>141</v>
       </c>
       <c r="I85" s="4" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="J85" s="4" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="K85" s="4" t="s">
         <v>7</v>
@@ -7239,14 +6528,10 @@
       <c r="Q85" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="S85" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="T85" s="5"/>
-      <c r="U85" s="3"/>
-      <c r="W85" s="3"/>
-    </row>
-    <row r="86" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R85" s="3"/>
+      <c r="T85" s="3"/>
+    </row>
+    <row r="86" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>145</v>
       </c>
@@ -7254,7 +6539,7 @@
         <v>142</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>399</v>
+        <v>389</v>
       </c>
       <c r="D86" s="4">
         <v>1</v>
@@ -7272,10 +6557,10 @@
         <v>36</v>
       </c>
       <c r="I86" s="4" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="J86" s="4" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="K86" s="4" t="s">
         <v>7</v>
@@ -7298,17 +6583,10 @@
       <c r="Q86" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="R86" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="S86" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="T86" s="5"/>
-      <c r="U86" s="3"/>
-      <c r="W86" s="3"/>
-    </row>
-    <row r="87" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R86" s="3"/>
+      <c r="T86" s="3"/>
+    </row>
+    <row r="87" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>12</v>
       </c>
@@ -7316,7 +6594,7 @@
         <v>213</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>396</v>
+        <v>386</v>
       </c>
       <c r="D87" s="4">
         <v>1</v>
@@ -7334,7 +6612,7 @@
         <v>13</v>
       </c>
       <c r="I87" s="4" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="J87" s="4" t="s">
         <v>38</v>
@@ -7360,34 +6638,27 @@
       <c r="Q87" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="R87" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="S87" s="5" t="s">
-        <v>259</v>
-      </c>
-      <c r="T87" s="5"/>
-      <c r="U87" s="3"/>
-      <c r="W87" s="3"/>
-    </row>
-    <row r="88" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="R87" s="3"/>
+      <c r="T87" s="3"/>
+    </row>
+    <row r="88" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>406</v>
+        <v>396</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>407</v>
+        <v>397</v>
       </c>
       <c r="G88" s="4" t="s">
         <v>99</v>
       </c>
       <c r="H88" s="4" t="s">
-        <v>408</v>
+        <v>398</v>
       </c>
       <c r="I88" s="4" t="s">
-        <v>409</v>
+        <v>399</v>
       </c>
       <c r="J88" s="4" t="s">
-        <v>410</v>
+        <v>400</v>
       </c>
       <c r="K88" s="4" t="s">
         <v>241</v>
@@ -7410,97 +6681,51 @@
       <c r="Q88" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="R88" s="5"/>
-      <c r="S88" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="T88" s="5" t="s">
-        <v>383</v>
-      </c>
-      <c r="U88" s="3"/>
-      <c r="W88" s="3"/>
+      <c r="R88" s="3"/>
+      <c r="T88" s="3"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="K1:K88">
-    <cfRule type="cellIs" dxfId="21" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="19" operator="equal">
       <formula>"q"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="20" operator="equal">
       <formula>"m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="21" operator="equal">
       <formula>"w"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="22" operator="equal">
       <formula>"d"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S89:S9963 P88">
-    <cfRule type="expression" dxfId="17" priority="18">
+  <conditionalFormatting sqref="P88">
+    <cfRule type="expression" dxfId="25" priority="18">
       <formula>#REF! &lt;&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H88">
-    <cfRule type="expression" dxfId="16" priority="17">
+    <cfRule type="expression" dxfId="24" priority="17">
       <formula>$G2="calc"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2:P88">
-    <cfRule type="expression" dxfId="15" priority="16">
+    <cfRule type="expression" dxfId="23" priority="16">
       <formula>AND($K2&lt;&gt;"d", $K2 &lt;&gt; "w", $K2 &lt;&gt; "m")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S2:S88">
-    <cfRule type="cellIs" dxfId="14" priority="3" operator="equal">
-      <formula>"core.exog.p"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="9" operator="equal">
-      <formula>"post.endog"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
-      <formula>"core.endog"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="14" operator="equal">
+  <conditionalFormatting sqref="Q2:Q88">
+    <cfRule type="cellIs" dxfId="22" priority="4" operator="equal">
       <formula>"none"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="15" operator="equal">
-      <formula>"core.exog"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q2:Q88">
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
-      <formula>"none"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="10" operator="equal">
       <formula>"dfm.q"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="11" operator="equal">
       <formula>"dfm.m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="12" operator="equal">
       <formula>"calc"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="T2:T88">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
-      <formula>"identity.ll"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
-      <formula>"estimated"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="3" priority="8">
-      <formula>AND($S2 &lt;&gt; "core.endog",$S2 &lt;&gt; "core.exog.p")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="R2:R88">
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
-      <formula>"calc"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="6" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="7" operator="equal">
-      <formula>"qual"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7533,33 +6758,33 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="B1" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="C1" t="s">
+        <v>258</v>
+      </c>
+      <c r="D1" t="s">
+        <v>259</v>
+      </c>
+      <c r="E1" t="s">
+        <v>260</v>
+      </c>
+      <c r="F1" t="s">
         <v>263</v>
-      </c>
-      <c r="D1" t="s">
-        <v>264</v>
-      </c>
-      <c r="E1" t="s">
-        <v>265</v>
-      </c>
-      <c r="F1" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="B2" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="C2" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="D2" t="s">
         <v>99</v>
@@ -7570,13 +6795,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
       <c r="B3" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="C3" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="D3" t="s">
         <v>99</v>
@@ -7587,13 +6812,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="B4" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="C4" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="D4" t="s">
         <v>99</v>
@@ -7604,13 +6829,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="B5" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="C5" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="D5" t="s">
         <v>99</v>
@@ -7621,13 +6846,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="B6" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="C6" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="D6" t="s">
         <v>99</v>
@@ -7638,13 +6863,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="B7" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C7" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="D7" t="s">
         <v>99</v>
@@ -7655,13 +6880,13 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="B8" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="C8" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="D8" t="s">
         <v>99</v>
@@ -7672,13 +6897,13 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="B9" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="C9" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="D9" t="s">
         <v>99</v>
@@ -7689,13 +6914,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="B10" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="C10" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="D10" t="s">
         <v>99</v>
@@ -7706,13 +6931,13 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="B11" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="C11" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="D11" t="s">
         <v>99</v>
@@ -7723,13 +6948,13 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="B12" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="C12" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="D12" t="s">
         <v>99</v>
@@ -7740,13 +6965,13 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="B13" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="C13" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="D13" t="s">
         <v>99</v>
@@ -7755,18 +6980,18 @@
         <v>465</v>
       </c>
       <c r="F13" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="B14" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="C14" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="D14" t="s">
         <v>99</v>
@@ -7777,13 +7002,13 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="B15" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="C15" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="D15" t="s">
         <v>99</v>
@@ -7794,7 +7019,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="B16" t="s">
         <v>27</v>
@@ -7806,18 +7031,18 @@
         <v>187</v>
       </c>
       <c r="F16" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="B17" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="C17" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="D17" t="s">
         <v>99</v>
@@ -7828,13 +7053,13 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
       <c r="B18" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
       <c r="C18" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="D18" t="s">
         <v>99</v>
@@ -7845,13 +7070,13 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="B19" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="C19" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="D19" t="s">
         <v>99</v>
@@ -7860,18 +7085,18 @@
         <v>341</v>
       </c>
       <c r="F19" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="B20" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="C20" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="D20" t="s">
         <v>99</v>
@@ -7882,13 +7107,13 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="B21" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="C21" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="D21" t="s">
         <v>99</v>
@@ -7899,13 +7124,13 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="B22" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="C22" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="D22" t="s">
         <v>99</v>
@@ -7914,18 +7139,18 @@
         <v>321</v>
       </c>
       <c r="F22" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="B23" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="C23" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="D23" t="s">
         <v>99</v>
@@ -7934,18 +7159,18 @@
         <v>374</v>
       </c>
       <c r="F23" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B24" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="C24" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="D24" t="s">
         <v>99</v>
@@ -7954,18 +7179,18 @@
         <v>351</v>
       </c>
       <c r="F24" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="B25" t="s">
         <v>167</v>
       </c>
       <c r="C25" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="D25" t="s">
         <v>99</v>
@@ -7976,10 +7201,10 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="B26" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="D26" t="s">
         <v>99</v>
@@ -7990,13 +7215,13 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="B27" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="C27" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="D27" t="s">
         <v>99</v>
@@ -8007,13 +7232,13 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="B28" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="C28" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="D28" t="s">
         <v>99</v>
@@ -8024,13 +7249,13 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
       <c r="B29" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="C29" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="D29" t="s">
         <v>99</v>
@@ -8041,13 +7266,13 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>414</v>
+        <v>404</v>
       </c>
       <c r="B30" t="s">
-        <v>415</v>
+        <v>405</v>
       </c>
       <c r="C30" t="s">
-        <v>416</v>
+        <v>406</v>
       </c>
       <c r="D30" t="s">
         <v>99</v>
@@ -8055,13 +7280,13 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
       <c r="B31" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="C31" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="D31" t="s">
         <v>99</v>
@@ -8072,13 +7297,13 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="B32" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="C32" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="D32" t="s">
         <v>99</v>
@@ -8089,13 +7314,13 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="B33" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
       <c r="C33" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="D33" t="s">
         <v>166</v>
@@ -8103,13 +7328,13 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>409</v>
+        <v>399</v>
       </c>
       <c r="B34" t="s">
-        <v>411</v>
+        <v>401</v>
       </c>
       <c r="C34" t="s">
-        <v>412</v>
+        <v>402</v>
       </c>
       <c r="D34" t="s">
         <v>99</v>
@@ -8120,13 +7345,13 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>421</v>
+        <v>411</v>
       </c>
       <c r="B35" t="s">
-        <v>419</v>
+        <v>409</v>
       </c>
       <c r="C35" t="s">
-        <v>422</v>
+        <v>412</v>
       </c>
       <c r="D35" t="s">
         <v>99</v>
@@ -8137,13 +7362,13 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>429</v>
+        <v>419</v>
       </c>
       <c r="B36" t="s">
-        <v>430</v>
+        <v>420</v>
       </c>
       <c r="C36" t="s">
-        <v>431</v>
+        <v>421</v>
       </c>
       <c r="E36">
         <v>25</v>

</xml_diff>

<commit_message>
Added variable to allow for minimum import date selection (v0.20)
</commit_message>
<xml_diff>
--- a/modules/nowcast-model/nowcast-model-inputs.xlsx
+++ b/modules/nowcast-model/nowcast-model-inputs.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\modules\nowcast-model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDB8B2C6-4899-4901-B9E7-23BECE986760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD42873B-9AAB-49F0-A9BC-3441CFA77FC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
   </bookViews>
   <sheets>
     <sheet name="variables" sheetId="12" r:id="rId1"/>
     <sheet name="releases" sheetId="11" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1428,7 +1427,7 @@
     <t>Banking</t>
   </si>
   <si>
-    <t>BTC-USD</t>
+    <t>CBBTCUSD</t>
   </si>
 </sst>
 </file>
@@ -1507,83 +1506,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="31">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7D7D"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1916,6 +1838,83 @@
         <scheme val="minor"/>
       </font>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7D7D"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -1941,30 +1940,30 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{4AECC335-00AC-41E6-A3CA-F63691B92F69}" name="Table13279" displayName="Table13279" ref="A1:R98" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{4AECC335-00AC-41E6-A3CA-F63691B92F69}" name="Table13279" displayName="Table13279" ref="A1:R98" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
   <autoFilter ref="A1:R98" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R98">
     <sortCondition ref="C1:C98"/>
   </sortState>
   <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{CA6DE630-5CD5-428A-8439-1A504496E546}" name="varname" dataDxfId="28"/>
-    <tableColumn id="9" xr3:uid="{62B19A4C-5AC5-4FBE-B49F-BB64B9102385}" name="fullname" dataDxfId="27"/>
-    <tableColumn id="15" xr3:uid="{D22B03C4-4AE3-48C2-A598-07C9E704433D}" name="dispgroup" dataDxfId="26"/>
-    <tableColumn id="24" xr3:uid="{FDF2E866-66A2-44DE-B360-10560B9D2BFE}" name="disprank" dataDxfId="25"/>
-    <tableColumn id="25" xr3:uid="{5C657D4D-8A66-4157-8DB5-145B21A2134C}" name="disptabs" dataDxfId="24"/>
-    <tableColumn id="31" xr3:uid="{BB6C6479-DCFC-4184-88B3-AEDE3CAC59A3}" name="disporder" dataDxfId="23"/>
-    <tableColumn id="6" xr3:uid="{660D69F6-B312-40A1-9E4C-CFF43DBEC0B3}" name="source" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{172B3803-5494-4C90-B939-5C2F79872038}" name="sckey" dataDxfId="21"/>
-    <tableColumn id="14" xr3:uid="{3D01EE11-409F-43C6-990A-ABD3232293C0}" name="relkey" dataDxfId="20"/>
-    <tableColumn id="12" xr3:uid="{814C0F50-71A5-4E9D-9399-51983A27304D}" name="units" dataDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{5F680C4B-D29A-4EFC-BE1D-FFAD04A6ECBF}" name="freq" dataDxfId="18"/>
-    <tableColumn id="10" xr3:uid="{ED9C9D35-83EF-4D33-B5A6-29714463F59D}" name="sa" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{4C279BEC-C29C-4B88-A87A-0A23F3DE4D9A}" name="st" dataDxfId="16"/>
-    <tableColumn id="13" xr3:uid="{4C82AECA-D40C-41E9-9170-45F127D67DD4}" name="d1" dataDxfId="15"/>
-    <tableColumn id="11" xr3:uid="{BCA31579-22E5-46AB-AC81-7237E8AE8CCD}" name="d2" dataDxfId="14"/>
-    <tableColumn id="16" xr3:uid="{5323D81D-334B-41E1-9C57-FB97D32790FE}" name="nc_dfm_input" dataDxfId="13"/>
-    <tableColumn id="17" xr3:uid="{136836AD-D381-4336-9040-09625567FE1C}" name="nc_method" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{3F173539-12EB-41F3-B70E-7885DB3C4CE4}" name="nc_input_reason" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{CA6DE630-5CD5-428A-8439-1A504496E546}" name="varname" dataDxfId="17"/>
+    <tableColumn id="9" xr3:uid="{62B19A4C-5AC5-4FBE-B49F-BB64B9102385}" name="fullname" dataDxfId="16"/>
+    <tableColumn id="15" xr3:uid="{D22B03C4-4AE3-48C2-A598-07C9E704433D}" name="dispgroup" dataDxfId="15"/>
+    <tableColumn id="24" xr3:uid="{FDF2E866-66A2-44DE-B360-10560B9D2BFE}" name="disprank" dataDxfId="14"/>
+    <tableColumn id="25" xr3:uid="{5C657D4D-8A66-4157-8DB5-145B21A2134C}" name="disptabs" dataDxfId="13"/>
+    <tableColumn id="31" xr3:uid="{BB6C6479-DCFC-4184-88B3-AEDE3CAC59A3}" name="disporder" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{660D69F6-B312-40A1-9E4C-CFF43DBEC0B3}" name="source" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{172B3803-5494-4C90-B939-5C2F79872038}" name="sckey" dataDxfId="10"/>
+    <tableColumn id="14" xr3:uid="{3D01EE11-409F-43C6-990A-ABD3232293C0}" name="relkey" dataDxfId="9"/>
+    <tableColumn id="12" xr3:uid="{814C0F50-71A5-4E9D-9399-51983A27304D}" name="units" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{5F680C4B-D29A-4EFC-BE1D-FFAD04A6ECBF}" name="freq" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{ED9C9D35-83EF-4D33-B5A6-29714463F59D}" name="sa" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{4C279BEC-C29C-4B88-A87A-0A23F3DE4D9A}" name="st" dataDxfId="5"/>
+    <tableColumn id="13" xr3:uid="{4C82AECA-D40C-41E9-9170-45F127D67DD4}" name="d1" dataDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{BCA31579-22E5-46AB-AC81-7237E8AE8CCD}" name="d2" dataDxfId="3"/>
+    <tableColumn id="16" xr3:uid="{5323D81D-334B-41E1-9C57-FB97D32790FE}" name="nc_dfm_input" dataDxfId="2"/>
+    <tableColumn id="17" xr3:uid="{136836AD-D381-4336-9040-09625567FE1C}" name="nc_method" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{3F173539-12EB-41F3-B70E-7885DB3C4CE4}" name="nc_input_reason" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2287,8 +2286,8 @@
   </sheetPr>
   <dimension ref="A1:T98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="L81" sqref="L81"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="M102" sqref="M102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5675,7 +5674,7 @@
         <v>246</v>
       </c>
       <c r="M63" s="4" t="s">
-        <v>367</v>
+        <v>442</v>
       </c>
       <c r="N63" s="4" t="s">
         <v>4</v>
@@ -7260,7 +7259,7 @@
         <v>462</v>
       </c>
       <c r="I92" s="4" t="s">
-        <v>345</v>
+        <v>386</v>
       </c>
       <c r="J92" s="4" t="s">
         <v>387</v>
@@ -7617,45 +7616,45 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="K1:K98">
-    <cfRule type="cellIs" dxfId="10" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="19" operator="equal">
       <formula>"q"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="20" operator="equal">
       <formula>"m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="21" operator="equal">
       <formula>"w"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="22" operator="equal">
       <formula>"d"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P94">
-    <cfRule type="expression" dxfId="6" priority="18">
+    <cfRule type="expression" dxfId="26" priority="18">
       <formula>#REF! &lt;&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H98">
-    <cfRule type="expression" dxfId="5" priority="17">
+    <cfRule type="expression" dxfId="25" priority="17">
       <formula>$G2="calc"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2:P98">
-    <cfRule type="expression" dxfId="4" priority="16">
+    <cfRule type="expression" dxfId="24" priority="16">
       <formula>AND($K2&lt;&gt;"d", $K2 &lt;&gt; "w", $K2 &lt;&gt; "m")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q98">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="4" operator="equal">
       <formula>"none"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="10" operator="equal">
       <formula>"dfm.q"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="11" operator="equal">
       <formula>"dfm.m"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="12" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added mortgage models (v0.20)
</commit_message>
<xml_diff>
--- a/modules/nowcast-model/nowcast-model-inputs.xlsx
+++ b/modules/nowcast-model/nowcast-model-inputs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charles\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\modules\nowcast-model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FEE3BE4-FB20-4D92-8E5C-60FB5F33055D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A845A1C-656C-4250-B7D2-FC5B9CFA7C99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
   </bookViews>
   <sheets>
     <sheet name="variables" sheetId="12" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1314" uniqueCount="454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1327" uniqueCount="459">
   <si>
     <t>gdp</t>
   </si>
@@ -751,9 +751,6 @@
   </si>
   <si>
     <t>CPIAUCSL</t>
-  </si>
-  <si>
-    <t>inf</t>
   </si>
   <si>
     <t>1-Year CPI Inflation</t>
@@ -1401,6 +1398,24 @@
   </si>
   <si>
     <t>CBBTCUSD</t>
+  </si>
+  <si>
+    <t>cpi0</t>
+  </si>
+  <si>
+    <t>pcepi0</t>
+  </si>
+  <si>
+    <t>1-Year PCEPI Inflation</t>
+  </si>
+  <si>
+    <t>BLS.PI</t>
+  </si>
+  <si>
+    <t>Import to calculate CPI</t>
+  </si>
+  <si>
+    <t>Import to calculate PCEPI</t>
   </si>
 </sst>
 </file>
@@ -1911,10 +1926,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{4AECC335-00AC-41E6-A3CA-F63691B92F69}" name="Table13279" displayName="Table13279" ref="A1:Q97" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
-  <autoFilter ref="A1:Q97" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q97">
-    <sortCondition ref="C1:C97"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{4AECC335-00AC-41E6-A3CA-F63691B92F69}" name="Table13279" displayName="Table13279" ref="A1:Q98" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
+  <autoFilter ref="A1:Q98" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q98">
+    <sortCondition ref="C1:C98"/>
   </sortState>
   <tableColumns count="17">
     <tableColumn id="1" xr3:uid="{CA6DE630-5CD5-428A-8439-1A504496E546}" name="varname" dataDxfId="27"/>
@@ -2239,10 +2254,10 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:T97"/>
+  <dimension ref="A1:T98"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="O59" sqref="O59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2276,13 +2291,13 @@
         <v>193</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>365</v>
-      </c>
       <c r="F1" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>97</v>
@@ -2291,7 +2306,7 @@
         <v>100</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>36</v>
@@ -2309,13 +2324,13 @@
         <v>196</v>
       </c>
       <c r="O1" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>245</v>
-      </c>
       <c r="Q1" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="R1" s="3"/>
       <c r="T1" s="3"/>
@@ -2328,7 +2343,7 @@
         <v>34</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D2" s="4">
         <v>3</v>
@@ -2346,10 +2361,10 @@
         <v>44</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>7</v>
@@ -2381,7 +2396,7 @@
         <v>141</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D3" s="4">
         <v>1</v>
@@ -2399,10 +2414,10 @@
         <v>138</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>7</v>
@@ -2434,7 +2449,7 @@
         <v>146</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D4" s="4">
         <v>1</v>
@@ -2452,10 +2467,10 @@
         <v>148</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>7</v>
@@ -2487,7 +2502,7 @@
         <v>145</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D5" s="4">
         <v>1</v>
@@ -2505,10 +2520,10 @@
         <v>147</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K5" s="4" t="s">
         <v>7</v>
@@ -2540,7 +2555,7 @@
         <v>136</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D6" s="4">
         <v>1</v>
@@ -2558,10 +2573,10 @@
         <v>139</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K6" s="4" t="s">
         <v>7</v>
@@ -2593,7 +2608,7 @@
         <v>140</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D7" s="4">
         <v>1</v>
@@ -2611,10 +2626,10 @@
         <v>35</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K7" s="4" t="s">
         <v>7</v>
@@ -2640,13 +2655,13 @@
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>354</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>355</v>
-      </c>
       <c r="C8" s="4" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D8" s="4">
         <v>2</v>
@@ -2661,22 +2676,22 @@
         <v>98</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="K8" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="M8" s="4" t="s">
         <v>241</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="M8" s="4" t="s">
-        <v>242</v>
       </c>
       <c r="N8" s="4" t="s">
         <v>192</v>
@@ -2693,13 +2708,13 @@
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D9" s="4">
         <v>2</v>
@@ -2717,19 +2732,19 @@
         <v>15</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="K9" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="M9" s="4" t="s">
         <v>241</v>
-      </c>
-      <c r="L9" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="M9" s="4" t="s">
-        <v>242</v>
       </c>
       <c r="N9" s="4" t="s">
         <v>192</v>
@@ -2752,7 +2767,7 @@
         <v>151</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D10" s="4">
         <v>1</v>
@@ -2770,7 +2785,7 @@
         <v>156</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="J10" s="4" t="s">
         <v>37</v>
@@ -2803,7 +2818,7 @@
         <v>153</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D11" s="4">
         <v>1</v>
@@ -2821,7 +2836,7 @@
         <v>157</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="J11" s="4" t="s">
         <v>37</v>
@@ -2854,7 +2869,7 @@
         <v>155</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D12" s="4">
         <v>1</v>
@@ -2872,7 +2887,7 @@
         <v>158</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="J12" s="4" t="s">
         <v>37</v>
@@ -2923,10 +2938,10 @@
         <v>2</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K13" s="4" t="s">
         <v>6</v>
@@ -2953,7 +2968,7 @@
         <v>33</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>22</v>
@@ -2974,10 +2989,10 @@
         <v>50</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K14" s="4" t="s">
         <v>6</v>
@@ -3025,10 +3040,10 @@
         <v>51</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K15" s="4" t="s">
         <v>6</v>
@@ -3076,10 +3091,10 @@
         <v>52</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K16" s="4" t="s">
         <v>6</v>
@@ -3127,10 +3142,10 @@
         <v>104</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K17" s="4" t="s">
         <v>6</v>
@@ -3178,10 +3193,10 @@
         <v>105</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K18" s="4" t="s">
         <v>6</v>
@@ -3229,10 +3244,10 @@
         <v>106</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K19" s="4" t="s">
         <v>6</v>
@@ -3280,10 +3295,10 @@
         <v>107</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K20" s="4" t="s">
         <v>6</v>
@@ -3331,10 +3346,10 @@
         <v>53</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K21" s="4" t="s">
         <v>6</v>
@@ -3382,10 +3397,10 @@
         <v>54</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K22" s="4" t="s">
         <v>6</v>
@@ -3433,10 +3448,10 @@
         <v>112</v>
       </c>
       <c r="I23" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J23" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K23" s="4" t="s">
         <v>6</v>
@@ -3484,10 +3499,10 @@
         <v>113</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K24" s="4" t="s">
         <v>6</v>
@@ -3535,10 +3550,10 @@
         <v>114</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K25" s="4" t="s">
         <v>6</v>
@@ -3586,10 +3601,10 @@
         <v>55</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J26" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K26" s="4" t="s">
         <v>6</v>
@@ -3637,10 +3652,10 @@
         <v>56</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K27" s="4" t="s">
         <v>6</v>
@@ -3688,10 +3703,10 @@
         <v>57</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K28" s="4" t="s">
         <v>6</v>
@@ -3739,10 +3754,10 @@
         <v>58</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J29" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K29" s="4" t="s">
         <v>6</v>
@@ -3790,10 +3805,10 @@
         <v>59</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K30" s="4" t="s">
         <v>6</v>
@@ -3841,10 +3856,10 @@
         <v>60</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K31" s="4" t="s">
         <v>6</v>
@@ -3892,10 +3907,10 @@
         <v>61</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K32" s="4" t="s">
         <v>6</v>
@@ -3943,10 +3958,10 @@
         <v>62</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K33" s="4" t="s">
         <v>6</v>
@@ -3994,10 +4009,10 @@
         <v>63</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K34" s="4" t="s">
         <v>6</v>
@@ -4045,10 +4060,10 @@
         <v>46</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K35" s="4" t="s">
         <v>6</v>
@@ -4096,10 +4111,10 @@
         <v>64</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K36" s="4" t="s">
         <v>6</v>
@@ -4147,10 +4162,10 @@
         <v>124</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K37" s="4" t="s">
         <v>6</v>
@@ -4198,10 +4213,10 @@
         <v>125</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K38" s="4" t="s">
         <v>6</v>
@@ -4249,10 +4264,10 @@
         <v>126</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J39" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K39" s="4" t="s">
         <v>6</v>
@@ -4300,10 +4315,10 @@
         <v>65</v>
       </c>
       <c r="I40" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K40" s="4" t="s">
         <v>6</v>
@@ -4351,16 +4366,16 @@
         <v>66</v>
       </c>
       <c r="I41" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K41" s="4" t="s">
         <v>6</v>
       </c>
       <c r="L41" s="4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="M41" s="4" t="s">
         <v>4</v>
@@ -4402,10 +4417,10 @@
         <v>67</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K42" s="4" t="s">
         <v>6</v>
@@ -4453,10 +4468,10 @@
         <v>102</v>
       </c>
       <c r="I43" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K43" s="4" t="s">
         <v>6</v>
@@ -4504,10 +4519,10 @@
         <v>131</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K44" s="4" t="s">
         <v>6</v>
@@ -4555,10 +4570,10 @@
         <v>132</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K45" s="4" t="s">
         <v>6</v>
@@ -4606,10 +4621,10 @@
         <v>101</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J46" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K46" s="4" t="s">
         <v>6</v>
@@ -4657,10 +4672,10 @@
         <v>133</v>
       </c>
       <c r="I47" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K47" s="4" t="s">
         <v>6</v>
@@ -4708,10 +4723,10 @@
         <v>134</v>
       </c>
       <c r="I48" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K48" s="4" t="s">
         <v>6</v>
@@ -4759,10 +4774,10 @@
         <v>68</v>
       </c>
       <c r="I49" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K49" s="4" t="s">
         <v>6</v>
@@ -4810,10 +4825,10 @@
         <v>69</v>
       </c>
       <c r="I50" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K50" s="4" t="s">
         <v>6</v>
@@ -4861,10 +4876,10 @@
         <v>70</v>
       </c>
       <c r="I51" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K51" s="4" t="s">
         <v>6</v>
@@ -4891,7 +4906,7 @@
         <v>8</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>217</v>
@@ -4912,7 +4927,7 @@
         <v>9</v>
       </c>
       <c r="I52" s="4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="J52" s="4" t="s">
         <v>40</v>
@@ -4941,10 +4956,10 @@
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>217</v>
@@ -4962,10 +4977,10 @@
         <v>98</v>
       </c>
       <c r="H53" s="4" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="I53" s="4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="J53" s="4" t="s">
         <v>40</v>
@@ -5018,7 +5033,7 @@
         <v>207</v>
       </c>
       <c r="I54" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J54" s="4" t="s">
         <v>219</v>
@@ -5027,7 +5042,7 @@
         <v>7</v>
       </c>
       <c r="L54" s="4" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="M54" s="4" t="s">
         <v>4</v>
@@ -5071,7 +5086,7 @@
         <v>218</v>
       </c>
       <c r="I55" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="J55" s="4" t="s">
         <v>219</v>
@@ -5080,7 +5095,7 @@
         <v>7</v>
       </c>
       <c r="L55" s="4" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="M55" s="4" t="s">
         <v>4</v>
@@ -5124,7 +5139,7 @@
         <v>224</v>
       </c>
       <c r="I56" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J56" s="4" t="s">
         <v>219</v>
@@ -5133,7 +5148,7 @@
         <v>7</v>
       </c>
       <c r="L56" s="4" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="M56" s="4" t="s">
         <v>4</v>
@@ -5153,10 +5168,10 @@
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="B57" s="3" t="s">
         <v>386</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>387</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>217</v>
@@ -5174,10 +5189,10 @@
         <v>98</v>
       </c>
       <c r="H57" s="4" t="s">
+        <v>387</v>
+      </c>
+      <c r="I57" s="4" t="s">
         <v>388</v>
-      </c>
-      <c r="I57" s="4" t="s">
-        <v>389</v>
       </c>
       <c r="J57" s="4" t="s">
         <v>40</v>
@@ -5206,10 +5221,10 @@
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>239</v>
+        <v>41</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>240</v>
+        <v>455</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>99</v>
@@ -5228,7 +5243,7 @@
       </c>
       <c r="H58" s="4"/>
       <c r="I58" s="4" t="s">
-        <v>324</v>
+        <v>456</v>
       </c>
       <c r="J58" s="4" t="s">
         <v>37</v>
@@ -5246,7 +5261,7 @@
         <v>192</v>
       </c>
       <c r="O58" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P58" s="5" t="s">
         <v>96</v>
@@ -5257,10 +5272,10 @@
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>41</v>
+        <v>236</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>43</v>
+        <v>239</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>99</v>
@@ -5275,25 +5290,23 @@
         <v>2</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="H59" s="4" t="s">
-        <v>42</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="H59" s="4"/>
       <c r="I59" s="4" t="s">
-        <v>336</v>
+        <v>323</v>
       </c>
       <c r="J59" s="4" t="s">
-        <v>371</v>
+        <v>37</v>
       </c>
       <c r="K59" s="4" t="s">
         <v>7</v>
       </c>
       <c r="L59" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M59" s="4" t="s">
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="N59" s="4" t="s">
         <v>192</v>
@@ -5310,16 +5323,16 @@
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>236</v>
+        <v>454</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>237</v>
+        <v>43</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>99</v>
       </c>
       <c r="D60" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E60" s="4">
         <v>1</v>
@@ -5331,19 +5344,19 @@
         <v>98</v>
       </c>
       <c r="H60" s="4" t="s">
-        <v>238</v>
+        <v>42</v>
       </c>
       <c r="I60" s="4" t="s">
-        <v>324</v>
+        <v>335</v>
       </c>
       <c r="J60" s="4" t="s">
-        <v>40</v>
+        <v>370</v>
       </c>
       <c r="K60" s="4" t="s">
         <v>7</v>
       </c>
       <c r="L60" s="4" t="s">
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="M60" s="4" t="s">
         <v>4</v>
@@ -5352,27 +5365,29 @@
         <v>192</v>
       </c>
       <c r="O60" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P60" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="Q60" s="6"/>
+      <c r="Q60" s="6" t="s">
+        <v>457</v>
+      </c>
       <c r="R60" s="3"/>
       <c r="T60" s="3"/>
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>440</v>
+        <v>453</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>441</v>
+        <v>237</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>99</v>
       </c>
       <c r="D61" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E61" s="4">
         <v>1</v>
@@ -5384,45 +5399,47 @@
         <v>98</v>
       </c>
       <c r="H61" s="4" t="s">
-        <v>442</v>
+        <v>238</v>
       </c>
       <c r="I61" s="4" t="s">
-        <v>443</v>
+        <v>323</v>
       </c>
       <c r="J61" s="4" t="s">
-        <v>446</v>
+        <v>40</v>
       </c>
       <c r="K61" s="4" t="s">
         <v>7</v>
       </c>
       <c r="L61" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M61" s="4" t="s">
         <v>4</v>
       </c>
       <c r="N61" s="4" t="s">
-        <v>4</v>
+        <v>192</v>
       </c>
       <c r="O61" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P61" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="Q61" s="7"/>
+      <c r="Q61" s="6" t="s">
+        <v>458</v>
+      </c>
       <c r="R61" s="3"/>
       <c r="T61" s="3"/>
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>447</v>
+        <v>439</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>210</v>
+        <v>440</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>367</v>
+        <v>99</v>
       </c>
       <c r="D62" s="4">
         <v>1</v>
@@ -5431,31 +5448,31 @@
         <v>1</v>
       </c>
       <c r="F62" s="4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G62" s="4" t="s">
         <v>98</v>
       </c>
       <c r="H62" s="4" t="s">
-        <v>12</v>
+        <v>441</v>
       </c>
       <c r="I62" s="4" t="s">
-        <v>319</v>
+        <v>442</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>37</v>
+        <v>445</v>
       </c>
       <c r="K62" s="4" t="s">
         <v>7</v>
       </c>
       <c r="L62" s="4" t="s">
-        <v>433</v>
+        <v>3</v>
       </c>
       <c r="M62" s="4" t="s">
         <v>4</v>
       </c>
       <c r="N62" s="4" t="s">
-        <v>192</v>
+        <v>4</v>
       </c>
       <c r="O62" s="5">
         <v>1</v>
@@ -5463,46 +5480,46 @@
       <c r="P62" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="Q62" s="6"/>
+      <c r="Q62" s="7"/>
       <c r="R62" s="3"/>
       <c r="T62" s="3"/>
     </row>
     <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>208</v>
+        <v>446</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D63" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E63" s="4">
         <v>1</v>
       </c>
       <c r="F63" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G63" s="4" t="s">
         <v>98</v>
       </c>
       <c r="H63" s="4" t="s">
-        <v>211</v>
+        <v>12</v>
       </c>
       <c r="I63" s="4" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>219</v>
+        <v>37</v>
       </c>
       <c r="K63" s="4" t="s">
         <v>7</v>
       </c>
       <c r="L63" s="4" t="s">
-        <v>3</v>
+        <v>432</v>
       </c>
       <c r="M63" s="4" t="s">
         <v>4</v>
@@ -5511,26 +5528,24 @@
         <v>192</v>
       </c>
       <c r="O63" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P63" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="Q63" s="6" t="s">
-        <v>405</v>
-      </c>
+      <c r="Q63" s="6"/>
       <c r="R63" s="3"/>
       <c r="T63" s="3"/>
     </row>
     <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>226</v>
+        <v>208</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>363</v>
+        <v>209</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D64" s="4">
         <v>3</v>
@@ -5539,16 +5554,16 @@
         <v>1</v>
       </c>
       <c r="F64" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G64" s="4" t="s">
         <v>98</v>
       </c>
       <c r="H64" s="4" t="s">
-        <v>227</v>
+        <v>211</v>
       </c>
       <c r="I64" s="4" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="J64" s="4" t="s">
         <v>219</v>
@@ -5566,24 +5581,26 @@
         <v>192</v>
       </c>
       <c r="O64" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P64" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="Q64" s="6"/>
+      <c r="Q64" s="6" t="s">
+        <v>404</v>
+      </c>
       <c r="R64" s="3"/>
       <c r="T64" s="3"/>
     </row>
     <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>391</v>
+        <v>226</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>392</v>
+        <v>362</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D65" s="4">
         <v>3</v>
@@ -5592,16 +5609,16 @@
         <v>1</v>
       </c>
       <c r="F65" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G65" s="4" t="s">
         <v>98</v>
       </c>
       <c r="H65" s="4" t="s">
-        <v>393</v>
+        <v>227</v>
       </c>
       <c r="I65" s="4" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="J65" s="4" t="s">
         <v>219</v>
@@ -5610,7 +5627,7 @@
         <v>7</v>
       </c>
       <c r="L65" s="4" t="s">
-        <v>242</v>
+        <v>3</v>
       </c>
       <c r="M65" s="4" t="s">
         <v>4</v>
@@ -5630,40 +5647,40 @@
     </row>
     <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>401</v>
+        <v>390</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>402</v>
+        <v>391</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D66" s="4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E66" s="4">
         <v>1</v>
       </c>
       <c r="F66" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G66" s="4" t="s">
         <v>98</v>
       </c>
       <c r="H66" s="4" t="s">
-        <v>403</v>
+        <v>392</v>
       </c>
       <c r="I66" s="4" t="s">
-        <v>319</v>
+        <v>328</v>
       </c>
       <c r="J66" s="4" t="s">
-        <v>404</v>
+        <v>219</v>
       </c>
       <c r="K66" s="4" t="s">
         <v>7</v>
       </c>
       <c r="L66" s="4" t="s">
-        <v>3</v>
+        <v>241</v>
       </c>
       <c r="M66" s="4" t="s">
         <v>4</v>
@@ -5683,13 +5700,13 @@
     </row>
     <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>16</v>
+        <v>400</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>26</v>
+        <v>401</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D67" s="4">
         <v>1</v>
@@ -5698,25 +5715,25 @@
         <v>1</v>
       </c>
       <c r="F67" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G67" s="4" t="s">
         <v>98</v>
       </c>
       <c r="H67" s="4" t="s">
-        <v>381</v>
+        <v>402</v>
       </c>
       <c r="I67" s="4" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>40</v>
+        <v>403</v>
       </c>
       <c r="K67" s="4" t="s">
-        <v>241</v>
+        <v>7</v>
       </c>
       <c r="L67" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M67" s="4" t="s">
         <v>4</v>
@@ -5725,10 +5742,10 @@
         <v>192</v>
       </c>
       <c r="O67" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P67" s="5" t="s">
-        <v>192</v>
+        <v>96</v>
       </c>
       <c r="Q67" s="6"/>
       <c r="R67" s="3"/>
@@ -5736,13 +5753,13 @@
     </row>
     <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D68" s="4">
         <v>1</v>
@@ -5751,22 +5768,22 @@
         <v>1</v>
       </c>
       <c r="F68" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G68" s="4" t="s">
         <v>98</v>
       </c>
       <c r="H68" s="4" t="s">
-        <v>20</v>
+        <v>380</v>
       </c>
       <c r="I68" s="4" t="s">
-        <v>335</v>
+        <v>320</v>
       </c>
       <c r="J68" s="4" t="s">
         <v>40</v>
       </c>
       <c r="K68" s="4" t="s">
-        <v>7</v>
+        <v>240</v>
       </c>
       <c r="L68" s="4" t="s">
         <v>4</v>
@@ -5778,7 +5795,7 @@
         <v>192</v>
       </c>
       <c r="O68" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P68" s="5" t="s">
         <v>192</v>
@@ -5789,13 +5806,13 @@
     </row>
     <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>231</v>
+        <v>19</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>232</v>
+        <v>39</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D69" s="4">
         <v>1</v>
@@ -5804,19 +5821,19 @@
         <v>1</v>
       </c>
       <c r="F69" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G69" s="4" t="s">
         <v>98</v>
       </c>
       <c r="H69" s="4" t="s">
-        <v>233</v>
+        <v>20</v>
       </c>
       <c r="I69" s="4" t="s">
-        <v>319</v>
+        <v>334</v>
       </c>
       <c r="J69" s="4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="K69" s="4" t="s">
         <v>7</v>
@@ -5834,7 +5851,7 @@
         <v>1</v>
       </c>
       <c r="P69" s="5" t="s">
-        <v>96</v>
+        <v>192</v>
       </c>
       <c r="Q69" s="6"/>
       <c r="R69" s="3"/>
@@ -5842,13 +5859,13 @@
     </row>
     <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>149</v>
+        <v>231</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>31</v>
+        <v>232</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>448</v>
+        <v>366</v>
       </c>
       <c r="D70" s="4">
         <v>1</v>
@@ -5857,28 +5874,28 @@
         <v>1</v>
       </c>
       <c r="F70" s="4">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G70" s="4" t="s">
         <v>98</v>
       </c>
       <c r="H70" s="4" t="s">
-        <v>32</v>
+        <v>233</v>
       </c>
       <c r="I70" s="4" t="s">
-        <v>311</v>
+        <v>318</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K70" s="4" t="s">
         <v>7</v>
       </c>
       <c r="L70" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M70" s="4" t="s">
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="N70" s="4" t="s">
         <v>192</v>
@@ -5895,34 +5912,34 @@
     </row>
     <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>426</v>
+        <v>149</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>423</v>
+        <v>31</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D71" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E71" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F71" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G71" s="4" t="s">
         <v>98</v>
       </c>
       <c r="H71" s="4" t="s">
-        <v>424</v>
+        <v>32</v>
       </c>
       <c r="I71" s="4" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="J71" s="4" t="s">
-        <v>425</v>
+        <v>40</v>
       </c>
       <c r="K71" s="4" t="s">
         <v>7</v>
@@ -5931,10 +5948,10 @@
         <v>3</v>
       </c>
       <c r="M71" s="4" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="N71" s="4" t="s">
-        <v>4</v>
+        <v>192</v>
       </c>
       <c r="O71" s="5">
         <v>1</v>
@@ -5942,19 +5959,19 @@
       <c r="P71" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="Q71" s="7"/>
+      <c r="Q71" s="6"/>
       <c r="R71" s="3"/>
       <c r="T71" s="3"/>
     </row>
     <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>428</v>
+        <v>422</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D72" s="4">
         <v>3</v>
@@ -5963,19 +5980,19 @@
         <v>2</v>
       </c>
       <c r="F72" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G72" s="4" t="s">
         <v>98</v>
       </c>
       <c r="H72" s="4" t="s">
-        <v>429</v>
+        <v>423</v>
       </c>
       <c r="I72" s="4" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="J72" s="4" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="K72" s="4" t="s">
         <v>7</v>
@@ -6001,13 +6018,13 @@
     </row>
     <row r="73" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D73" s="4">
         <v>3</v>
@@ -6016,19 +6033,19 @@
         <v>2</v>
       </c>
       <c r="F73" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G73" s="4" t="s">
         <v>98</v>
       </c>
       <c r="H73" s="4" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="I73" s="4" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="J73" s="4" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="K73" s="4" t="s">
         <v>7</v>
@@ -6054,46 +6071,46 @@
     </row>
     <row r="74" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>220</v>
+        <v>429</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>225</v>
+        <v>430</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D74" s="4">
+        <v>3</v>
+      </c>
+      <c r="E74" s="4">
         <v>2</v>
       </c>
-      <c r="E74" s="4">
-        <v>1</v>
-      </c>
       <c r="F74" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G74" s="4" t="s">
         <v>98</v>
       </c>
       <c r="H74" s="4" t="s">
-        <v>221</v>
+        <v>431</v>
       </c>
       <c r="I74" s="4" t="s">
-        <v>330</v>
+        <v>310</v>
       </c>
       <c r="J74" s="4" t="s">
-        <v>370</v>
+        <v>424</v>
       </c>
       <c r="K74" s="4" t="s">
         <v>7</v>
       </c>
       <c r="L74" s="4" t="s">
-        <v>242</v>
+        <v>3</v>
       </c>
       <c r="M74" s="4" t="s">
         <v>4</v>
       </c>
       <c r="N74" s="4" t="s">
-        <v>192</v>
+        <v>4</v>
       </c>
       <c r="O74" s="5">
         <v>1</v>
@@ -6101,19 +6118,19 @@
       <c r="P74" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="Q74" s="6"/>
+      <c r="Q74" s="7"/>
       <c r="R74" s="3"/>
       <c r="T74" s="3"/>
     </row>
     <row r="75" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>434</v>
+        <v>220</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>435</v>
+        <v>225</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D75" s="4">
         <v>2</v>
@@ -6122,25 +6139,25 @@
         <v>1</v>
       </c>
       <c r="F75" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G75" s="4" t="s">
         <v>98</v>
       </c>
       <c r="H75" s="4" t="s">
-        <v>436</v>
+        <v>221</v>
       </c>
       <c r="I75" s="4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="J75" s="4" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="K75" s="4" t="s">
         <v>7</v>
       </c>
       <c r="L75" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="M75" s="4" t="s">
         <v>4</v>
@@ -6160,40 +6177,40 @@
     </row>
     <row r="76" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>212</v>
+        <v>433</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>213</v>
+        <v>434</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D76" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E76" s="4">
         <v>1</v>
       </c>
       <c r="F76" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G76" s="4" t="s">
         <v>98</v>
       </c>
       <c r="H76" s="4" t="s">
-        <v>214</v>
+        <v>435</v>
       </c>
       <c r="I76" s="4" t="s">
-        <v>315</v>
+        <v>329</v>
       </c>
       <c r="J76" s="4" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="K76" s="4" t="s">
         <v>7</v>
       </c>
       <c r="L76" s="4" t="s">
-        <v>3</v>
+        <v>241</v>
       </c>
       <c r="M76" s="4" t="s">
         <v>4</v>
@@ -6213,13 +6230,13 @@
     </row>
     <row r="77" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>394</v>
+        <v>212</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>395</v>
+        <v>213</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D77" s="4">
         <v>1</v>
@@ -6228,25 +6245,25 @@
         <v>1</v>
       </c>
       <c r="F77" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G77" s="4" t="s">
         <v>98</v>
       </c>
       <c r="H77" s="4" t="s">
-        <v>396</v>
+        <v>214</v>
       </c>
       <c r="I77" s="4" t="s">
-        <v>397</v>
+        <v>314</v>
       </c>
       <c r="J77" s="4" t="s">
-        <v>400</v>
+        <v>369</v>
       </c>
       <c r="K77" s="4" t="s">
         <v>7</v>
       </c>
       <c r="L77" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M77" s="4" t="s">
         <v>4</v>
@@ -6266,13 +6283,13 @@
     </row>
     <row r="78" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>412</v>
+        <v>393</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>413</v>
+        <v>394</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D78" s="4">
         <v>1</v>
@@ -6281,19 +6298,19 @@
         <v>1</v>
       </c>
       <c r="F78" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G78" s="4" t="s">
         <v>98</v>
       </c>
       <c r="H78" s="4" t="s">
-        <v>414</v>
+        <v>395</v>
       </c>
       <c r="I78" s="4" t="s">
-        <v>311</v>
+        <v>396</v>
       </c>
       <c r="J78" s="4" t="s">
-        <v>37</v>
+        <v>399</v>
       </c>
       <c r="K78" s="4" t="s">
         <v>7</v>
@@ -6319,13 +6336,13 @@
     </row>
     <row r="79" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>406</v>
+        <v>411</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>407</v>
+        <v>412</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>408</v>
+        <v>447</v>
       </c>
       <c r="D79" s="4">
         <v>1</v>
@@ -6334,22 +6351,22 @@
         <v>1</v>
       </c>
       <c r="F79" s="4">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="G79" s="4" t="s">
         <v>98</v>
       </c>
       <c r="H79" s="4" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="I79" s="4" t="s">
-        <v>322</v>
+        <v>310</v>
       </c>
       <c r="J79" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K79" s="4" t="s">
-        <v>235</v>
+        <v>7</v>
       </c>
       <c r="L79" s="4" t="s">
         <v>4</v>
@@ -6372,13 +6389,13 @@
     </row>
     <row r="80" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D80" s="4">
         <v>1</v>
@@ -6387,22 +6404,22 @@
         <v>1</v>
       </c>
       <c r="F80" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G80" s="4" t="s">
         <v>98</v>
       </c>
       <c r="H80" s="4" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="I80" s="4" t="s">
-        <v>338</v>
+        <v>321</v>
       </c>
       <c r="J80" s="4" t="s">
         <v>40</v>
       </c>
       <c r="K80" s="4" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="L80" s="4" t="s">
         <v>4</v>
@@ -6425,13 +6442,13 @@
     </row>
     <row r="81" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>422</v>
+        <v>408</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>418</v>
+        <v>409</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D81" s="4">
         <v>1</v>
@@ -6440,22 +6457,22 @@
         <v>1</v>
       </c>
       <c r="F81" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G81" s="4" t="s">
         <v>98</v>
       </c>
       <c r="H81" s="4" t="s">
-        <v>419</v>
+        <v>410</v>
       </c>
       <c r="I81" s="4" t="s">
-        <v>325</v>
+        <v>337</v>
       </c>
       <c r="J81" s="4" t="s">
         <v>40</v>
       </c>
       <c r="K81" s="4" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="L81" s="4" t="s">
         <v>4</v>
@@ -6481,10 +6498,10 @@
         <v>421</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D82" s="4">
         <v>1</v>
@@ -6493,16 +6510,16 @@
         <v>1</v>
       </c>
       <c r="F82" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G82" s="4" t="s">
         <v>98</v>
       </c>
       <c r="H82" s="4" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="I82" s="4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="J82" s="4" t="s">
         <v>40</v>
@@ -6531,40 +6548,40 @@
     </row>
     <row r="83" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>11</v>
+        <v>420</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>24</v>
+        <v>419</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>451</v>
+        <v>407</v>
       </c>
       <c r="D83" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E83" s="4">
         <v>1</v>
       </c>
       <c r="F83" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G83" s="4" t="s">
         <v>98</v>
       </c>
       <c r="H83" s="4" t="s">
-        <v>10</v>
+        <v>416</v>
       </c>
       <c r="I83" s="4" t="s">
-        <v>318</v>
+        <v>324</v>
       </c>
       <c r="J83" s="4" t="s">
-        <v>374</v>
+        <v>40</v>
       </c>
       <c r="K83" s="4" t="s">
-        <v>7</v>
+        <v>235</v>
       </c>
       <c r="L83" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M83" s="4" t="s">
         <v>4</v>
@@ -6584,34 +6601,34 @@
     </row>
     <row r="84" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D84" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E84" s="4">
         <v>1</v>
       </c>
       <c r="F84" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G84" s="4" t="s">
         <v>98</v>
       </c>
       <c r="H84" s="4" t="s">
-        <v>366</v>
+        <v>10</v>
       </c>
       <c r="I84" s="4" t="s">
-        <v>334</v>
+        <v>317</v>
       </c>
       <c r="J84" s="4" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="K84" s="4" t="s">
         <v>7</v>
@@ -6620,7 +6637,7 @@
         <v>3</v>
       </c>
       <c r="M84" s="4" t="s">
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="N84" s="4" t="s">
         <v>192</v>
@@ -6637,10 +6654,10 @@
     </row>
     <row r="85" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C85" s="4" t="s">
         <v>450</v>
@@ -6652,28 +6669,28 @@
         <v>1</v>
       </c>
       <c r="F85" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G85" s="4" t="s">
         <v>98</v>
       </c>
       <c r="H85" s="4" t="s">
-        <v>30</v>
+        <v>365</v>
       </c>
       <c r="I85" s="4" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="J85" s="4" t="s">
-        <v>40</v>
+        <v>369</v>
       </c>
       <c r="K85" s="4" t="s">
         <v>7</v>
       </c>
       <c r="L85" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M85" s="4" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="N85" s="4" t="s">
         <v>192</v>
@@ -6690,13 +6707,13 @@
     </row>
     <row r="86" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>199</v>
+        <v>28</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>343</v>
+        <v>29</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D86" s="4">
         <v>1</v>
@@ -6705,13 +6722,13 @@
         <v>1</v>
       </c>
       <c r="F86" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G86" s="4" t="s">
         <v>98</v>
       </c>
       <c r="H86" s="4" t="s">
-        <v>342</v>
+        <v>30</v>
       </c>
       <c r="I86" s="4" t="s">
         <v>328</v>
@@ -6735,7 +6752,7 @@
         <v>1</v>
       </c>
       <c r="P86" s="5" t="s">
-        <v>192</v>
+        <v>96</v>
       </c>
       <c r="Q86" s="6"/>
       <c r="R86" s="3"/>
@@ -6743,13 +6760,13 @@
     </row>
     <row r="87" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>204</v>
+        <v>342</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D87" s="4">
         <v>1</v>
@@ -6758,16 +6775,16 @@
         <v>1</v>
       </c>
       <c r="F87" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G87" s="4" t="s">
         <v>98</v>
       </c>
       <c r="H87" s="4" t="s">
-        <v>159</v>
+        <v>341</v>
       </c>
       <c r="I87" s="4" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="J87" s="4" t="s">
         <v>40</v>
@@ -6796,13 +6813,13 @@
     </row>
     <row r="88" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D88" s="4">
         <v>1</v>
@@ -6811,16 +6828,16 @@
         <v>1</v>
       </c>
       <c r="F88" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G88" s="4" t="s">
         <v>98</v>
       </c>
       <c r="H88" s="4" t="s">
-        <v>203</v>
+        <v>159</v>
       </c>
       <c r="I88" s="4" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="J88" s="4" t="s">
         <v>40</v>
@@ -6849,13 +6866,13 @@
     </row>
     <row r="89" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>13</v>
+        <v>201</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>25</v>
+        <v>202</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>368</v>
+        <v>449</v>
       </c>
       <c r="D89" s="4">
         <v>1</v>
@@ -6864,37 +6881,37 @@
         <v>1</v>
       </c>
       <c r="F89" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G89" s="4" t="s">
-        <v>164</v>
+        <v>98</v>
       </c>
       <c r="H89" s="4" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="I89" s="4" t="s">
-        <v>339</v>
+        <v>326</v>
       </c>
       <c r="J89" s="4" t="s">
         <v>40</v>
       </c>
       <c r="K89" s="4" t="s">
-        <v>235</v>
+        <v>7</v>
       </c>
       <c r="L89" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M89" s="4" t="s">
-        <v>242</v>
+        <v>4</v>
       </c>
       <c r="N89" s="4" t="s">
-        <v>4</v>
+        <v>192</v>
       </c>
       <c r="O89" s="5">
         <v>1</v>
       </c>
       <c r="P89" s="5" t="s">
-        <v>96</v>
+        <v>192</v>
       </c>
       <c r="Q89" s="6"/>
       <c r="R89" s="3"/>
@@ -6902,13 +6919,13 @@
     </row>
     <row r="90" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>437</v>
+        <v>13</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>438</v>
+        <v>25</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D90" s="4">
         <v>1</v>
@@ -6917,16 +6934,16 @@
         <v>1</v>
       </c>
       <c r="F90" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G90" s="4" t="s">
         <v>164</v>
       </c>
       <c r="H90" s="4" t="s">
-        <v>439</v>
+        <v>197</v>
       </c>
       <c r="I90" s="4" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="J90" s="4" t="s">
         <v>40</v>
@@ -6938,7 +6955,7 @@
         <v>3</v>
       </c>
       <c r="M90" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="N90" s="4" t="s">
         <v>4</v>
@@ -6955,34 +6972,34 @@
     </row>
     <row r="91" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>375</v>
+        <v>436</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>376</v>
+        <v>437</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D91" s="4">
+        <v>1</v>
+      </c>
+      <c r="E91" s="4">
+        <v>1</v>
+      </c>
+      <c r="F91" s="4">
         <v>2</v>
       </c>
-      <c r="E91" s="4">
-        <v>1</v>
-      </c>
-      <c r="F91" s="4">
-        <v>3</v>
-      </c>
       <c r="G91" s="4" t="s">
-        <v>98</v>
+        <v>164</v>
       </c>
       <c r="H91" s="4" t="s">
-        <v>453</v>
+        <v>438</v>
       </c>
       <c r="I91" s="4" t="s">
-        <v>377</v>
+        <v>338</v>
       </c>
       <c r="J91" s="4" t="s">
-        <v>378</v>
+        <v>40</v>
       </c>
       <c r="K91" s="4" t="s">
         <v>235</v>
@@ -6991,13 +7008,13 @@
         <v>3</v>
       </c>
       <c r="M91" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="N91" s="4" t="s">
         <v>4</v>
       </c>
       <c r="O91" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P91" s="5" t="s">
         <v>96</v>
@@ -7008,13 +7025,13 @@
     </row>
     <row r="92" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>14</v>
+        <v>374</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>23</v>
+        <v>375</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D92" s="4">
         <v>2</v>
@@ -7023,34 +7040,34 @@
         <v>1</v>
       </c>
       <c r="F92" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G92" s="4" t="s">
-        <v>164</v>
+        <v>98</v>
       </c>
       <c r="H92" s="4" t="s">
-        <v>198</v>
+        <v>452</v>
       </c>
       <c r="I92" s="4" t="s">
-        <v>339</v>
+        <v>376</v>
       </c>
       <c r="J92" s="4" t="s">
-        <v>40</v>
+        <v>377</v>
       </c>
       <c r="K92" s="4" t="s">
         <v>235</v>
       </c>
       <c r="L92" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M92" s="4" t="s">
-        <v>4</v>
+        <v>241</v>
       </c>
       <c r="N92" s="4" t="s">
-        <v>192</v>
+        <v>4</v>
       </c>
       <c r="O92" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P92" s="5" t="s">
         <v>96</v>
@@ -7061,13 +7078,13 @@
     </row>
     <row r="93" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>344</v>
+        <v>14</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>352</v>
+        <v>23</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D93" s="4">
         <v>2</v>
@@ -7076,16 +7093,16 @@
         <v>1</v>
       </c>
       <c r="F93" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G93" s="4" t="s">
         <v>164</v>
       </c>
       <c r="H93" s="4" t="s">
-        <v>345</v>
+        <v>198</v>
       </c>
       <c r="I93" s="4" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="J93" s="4" t="s">
         <v>40</v>
@@ -7094,13 +7111,13 @@
         <v>235</v>
       </c>
       <c r="L93" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M93" s="4" t="s">
-        <v>242</v>
+        <v>4</v>
       </c>
       <c r="N93" s="4" t="s">
-        <v>4</v>
+        <v>192</v>
       </c>
       <c r="O93" s="5">
         <v>1</v>
@@ -7114,13 +7131,13 @@
     </row>
     <row r="94" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="B94" s="3" t="s">
         <v>351</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D94" s="4">
         <v>2</v>
@@ -7129,16 +7146,16 @@
         <v>1</v>
       </c>
       <c r="F94" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G94" s="4" t="s">
         <v>164</v>
       </c>
       <c r="H94" s="4" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="I94" s="4" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="J94" s="4" t="s">
         <v>40</v>
@@ -7150,7 +7167,7 @@
         <v>3</v>
       </c>
       <c r="M94" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="N94" s="4" t="s">
         <v>4</v>
@@ -7163,18 +7180,17 @@
       </c>
       <c r="Q94" s="6"/>
       <c r="R94" s="3"/>
-      <c r="S94" s="4"/>
       <c r="T94" s="3"/>
     </row>
     <row r="95" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>228</v>
+        <v>345</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>229</v>
+        <v>350</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D95" s="4">
         <v>2</v>
@@ -7183,31 +7199,31 @@
         <v>1</v>
       </c>
       <c r="F95" s="4">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G95" s="4" t="s">
-        <v>98</v>
+        <v>164</v>
       </c>
       <c r="H95" s="4" t="s">
-        <v>230</v>
+        <v>346</v>
       </c>
       <c r="I95" s="4" t="s">
-        <v>331</v>
+        <v>338</v>
       </c>
       <c r="J95" s="4" t="s">
-        <v>373</v>
+        <v>40</v>
       </c>
       <c r="K95" s="4" t="s">
         <v>235</v>
       </c>
       <c r="L95" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M95" s="4" t="s">
-        <v>4</v>
+        <v>241</v>
       </c>
       <c r="N95" s="4" t="s">
-        <v>192</v>
+        <v>4</v>
       </c>
       <c r="O95" s="5">
         <v>1</v>
@@ -7222,34 +7238,34 @@
     </row>
     <row r="96" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>17</v>
+        <v>228</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>27</v>
+        <v>229</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D96" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E96" s="4">
         <v>1</v>
       </c>
       <c r="F96" s="4">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G96" s="4" t="s">
-        <v>164</v>
+        <v>98</v>
       </c>
       <c r="H96" s="4" t="s">
-        <v>385</v>
+        <v>230</v>
       </c>
       <c r="I96" s="4" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="J96" s="4" t="s">
-        <v>40</v>
+        <v>372</v>
       </c>
       <c r="K96" s="4" t="s">
         <v>235</v>
@@ -7264,7 +7280,7 @@
         <v>192</v>
       </c>
       <c r="O96" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P96" s="5" t="s">
         <v>96</v>
@@ -7276,31 +7292,31 @@
     </row>
     <row r="97" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>348</v>
+        <v>17</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>350</v>
+        <v>27</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D97" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E97" s="4">
         <v>1</v>
       </c>
       <c r="F97" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G97" s="4" t="s">
         <v>164</v>
       </c>
       <c r="H97" s="4" t="s">
-        <v>349</v>
+        <v>384</v>
       </c>
       <c r="I97" s="4" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="J97" s="4" t="s">
         <v>40</v>
@@ -7309,16 +7325,16 @@
         <v>235</v>
       </c>
       <c r="L97" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M97" s="4" t="s">
-        <v>242</v>
+        <v>4</v>
       </c>
       <c r="N97" s="4" t="s">
-        <v>4</v>
+        <v>192</v>
       </c>
       <c r="O97" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P97" s="5" t="s">
         <v>96</v>
@@ -7328,8 +7344,62 @@
       <c r="S97" s="4"/>
       <c r="T97" s="3"/>
     </row>
+    <row r="98" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="C98" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="D98" s="4">
+        <v>2</v>
+      </c>
+      <c r="E98" s="4">
+        <v>1</v>
+      </c>
+      <c r="F98" s="4">
+        <v>9</v>
+      </c>
+      <c r="G98" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="H98" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="I98" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="J98" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K98" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="L98" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="M98" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="N98" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="O98" s="5">
+        <v>1</v>
+      </c>
+      <c r="P98" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q98" s="6"/>
+      <c r="R98" s="3"/>
+      <c r="S98" s="4"/>
+      <c r="T98" s="3"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="K1:K97">
+  <conditionalFormatting sqref="K1:K98">
     <cfRule type="cellIs" dxfId="10" priority="19" operator="equal">
       <formula>"q"</formula>
     </cfRule>
@@ -7343,22 +7413,22 @@
       <formula>"d"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O93">
+  <conditionalFormatting sqref="O94">
     <cfRule type="expression" dxfId="6" priority="18">
       <formula>#REF! &lt;&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H97">
+  <conditionalFormatting sqref="H2:H98">
     <cfRule type="expression" dxfId="5" priority="17">
       <formula>$G2="calc"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O2:O97">
+  <conditionalFormatting sqref="O2:O98">
     <cfRule type="expression" dxfId="4" priority="16">
       <formula>AND($K2&lt;&gt;"d", $K2 &lt;&gt; "w", $K2 &lt;&gt; "m")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P2:P97">
+  <conditionalFormatting sqref="P2:P98">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"none"</formula>
     </cfRule>
@@ -7404,33 +7474,33 @@
   <sheetData>
     <row r="1" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>249</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>248</v>
-      </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="10" t="s">
         <v>250</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="E1" s="10" t="s">
         <v>251</v>
       </c>
-      <c r="E1" s="10" t="s">
-        <v>252</v>
-      </c>
       <c r="F1" s="10" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B2" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>253</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>254</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>98</v>
@@ -7442,13 +7512,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>98</v>
@@ -7460,13 +7530,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>98</v>
@@ -7478,13 +7548,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>98</v>
@@ -7496,13 +7566,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>98</v>
@@ -7514,13 +7584,13 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D7" s="9" t="s">
         <v>98</v>
@@ -7532,13 +7602,13 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>98</v>
@@ -7550,13 +7620,13 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>98</v>
@@ -7568,13 +7638,13 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>98</v>
@@ -7586,13 +7656,13 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>98</v>
@@ -7604,13 +7674,13 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>98</v>
@@ -7622,13 +7692,13 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>98</v>
@@ -7640,13 +7710,13 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>98</v>
@@ -7658,7 +7728,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>26</v>
@@ -7671,18 +7741,18 @@
         <v>187</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D16" s="9" t="s">
         <v>98</v>
@@ -7694,13 +7764,13 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B17" s="9" t="s">
+        <v>331</v>
+      </c>
+      <c r="C17" s="9" t="s">
         <v>332</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>333</v>
       </c>
       <c r="D17" s="9" t="s">
         <v>98</v>
@@ -7712,13 +7782,13 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D18" s="9" t="s">
         <v>98</v>
@@ -7727,18 +7797,18 @@
         <v>341</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D19" s="9" t="s">
         <v>98</v>
@@ -7750,13 +7820,13 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D20" s="9" t="s">
         <v>98</v>
@@ -7768,13 +7838,13 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D21" s="9" t="s">
         <v>98</v>
@@ -7783,18 +7853,18 @@
         <v>321</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D22" s="9" t="s">
         <v>98</v>
@@ -7803,18 +7873,18 @@
         <v>374</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D23" s="9" t="s">
         <v>98</v>
@@ -7823,15 +7893,15 @@
         <v>351</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C24" s="9"/>
       <c r="D24" s="9" t="s">
@@ -7844,13 +7914,13 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D25" s="9" t="s">
         <v>98</v>
@@ -7862,13 +7932,13 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D26" s="9" t="s">
         <v>98</v>
@@ -7880,13 +7950,13 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D27" s="9" t="s">
         <v>98</v>
@@ -7898,13 +7968,13 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
+        <v>381</v>
+      </c>
+      <c r="B28" s="9" t="s">
         <v>382</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="C28" s="9" t="s">
         <v>383</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>384</v>
       </c>
       <c r="D28" s="9" t="s">
         <v>98</v>
@@ -7914,13 +7984,13 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D29" s="9" t="s">
         <v>98</v>
@@ -7932,13 +8002,13 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D30" s="8" t="s">
         <v>98</v>
@@ -7949,13 +8019,13 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
+        <v>338</v>
+      </c>
+      <c r="B31" s="8" t="s">
         <v>339</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="C31" s="8" t="s">
         <v>340</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>341</v>
       </c>
       <c r="D31" s="8" t="s">
         <v>164</v>
@@ -7963,13 +8033,13 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B32" s="8" t="s">
+        <v>378</v>
+      </c>
+      <c r="C32" s="8" t="s">
         <v>379</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>380</v>
       </c>
       <c r="D32" s="8" t="s">
         <v>98</v>
@@ -7980,13 +8050,13 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="C33" s="8" t="s">
         <v>389</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>387</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>390</v>
       </c>
       <c r="D33" s="8" t="s">
         <v>98</v>
@@ -7997,13 +8067,13 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="B34" s="8" t="s">
         <v>397</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="C34" s="8" t="s">
         <v>398</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>399</v>
       </c>
       <c r="D34" s="8" t="s">
         <v>98</v>
@@ -8014,13 +8084,13 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
+        <v>442</v>
+      </c>
+      <c r="B35" s="8" t="s">
         <v>443</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="C35" s="8" t="s">
         <v>444</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>445</v>
       </c>
       <c r="D35" s="8" t="s">
         <v>98</v>

</xml_diff>